<commit_message>
updated mac version to 0.0.0.0.9
</commit_message>
<xml_diff>
--- a/examples/vpc.xlsx
+++ b/examples/vpc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jww/Developer/python/terraformer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F294152E-0914-0B45-AAA5-65420FFE1183}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D834777-CACF-2748-8E4E-E366241AEAA3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4740" yWindow="460" windowWidth="25600" windowHeight="14680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38500" yWindow="-17420" windowWidth="25600" windowHeight="14680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="vpc" sheetId="6" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="112">
   <si>
     <t>public_gateway</t>
   </si>
@@ -185,12 +185,6 @@
     <t>vsi2nic0</t>
   </si>
   <si>
-    <t>vsi3nic0</t>
-  </si>
-  <si>
-    <t>vsi4nic0</t>
-  </si>
-  <si>
     <t>create_timeout</t>
   </si>
   <si>
@@ -218,9 +212,6 @@
     <t>*group_name</t>
   </si>
   <si>
-    <t>vsi1nic1:subnet2:sg1:fip2;vsi1nic2:subnet2:sg2</t>
-  </si>
-  <si>
     <t>10.240.0.0/24</t>
   </si>
   <si>
@@ -245,12 +236,6 @@
     <t>vsi2</t>
   </si>
   <si>
-    <t>vsi3</t>
-  </si>
-  <si>
-    <t>vsi4</t>
-  </si>
-  <si>
     <t>key1</t>
   </si>
   <si>
@@ -384,6 +369,9 @@
   </si>
   <si>
     <t>Balanced 62 vCPUs x 248GB RAM (Gen 1)</t>
+  </si>
+  <si>
+    <t>volume2</t>
   </si>
 </sst>
 </file>
@@ -1355,8 +1343,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{3F1E4605-7351-6A4A-9807-A10DCEAD79B7}" name="Table7" displayName="Table7" ref="A1:Q5" totalsRowShown="0" headerRowDxfId="52" dataDxfId="51">
-  <autoFilter ref="A1:Q5" xr:uid="{4F0FA061-E3B2-AB4E-A276-92C803DED60C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{3F1E4605-7351-6A4A-9807-A10DCEAD79B7}" name="Table7" displayName="Table7" ref="A1:Q3" totalsRowShown="0" headerRowDxfId="52" dataDxfId="51">
+  <autoFilter ref="A1:Q3" xr:uid="{4F0FA061-E3B2-AB4E-A276-92C803DED60C}"/>
   <tableColumns count="17">
     <tableColumn id="1" xr3:uid="{B447E9AB-445F-0242-8396-EEAA92074797}" name="*name" dataDxfId="50"/>
     <tableColumn id="2" xr3:uid="{E6843232-FC96-094F-809F-D9A2D9A3F5CB}" name="*zone" dataDxfId="49"/>
@@ -1381,8 +1369,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C451A855-5250-674B-8039-E23EC3348E96}" name="Table11" displayName="Table11" ref="A1:J2" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
-  <autoFilter ref="A1:J2" xr:uid="{8CD156A6-A66F-1245-BCD2-9FAE26A0A77C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C451A855-5250-674B-8039-E23EC3348E96}" name="Table11" displayName="Table11" ref="A1:J3" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
+  <autoFilter ref="A1:J3" xr:uid="{8CD156A6-A66F-1245-BCD2-9FAE26A0A77C}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{CDC18A34-D228-8E41-90CD-62AD9ACAF229}" name="*name" dataDxfId="31"/>
     <tableColumn id="2" xr3:uid="{480E110A-7DA0-1A46-B19A-DAB8291BA972}" name="*zone" dataDxfId="30"/>
@@ -1741,21 +1729,21 @@
         <v>40</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B2" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="G2" s="14"/>
       <c r="H2" s="14"/>
@@ -1818,50 +1806,50 @@
         <v>0</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>24</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -1903,7 +1891,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69A31708-3A2C-4ADA-B3E5-8A1B18923F2A}">
-  <dimension ref="A1:Q5"/>
+  <dimension ref="A1:Q3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1934,10 +1922,10 @@
         <v>2</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="G1" s="7" t="s">
         <v>8</v>
@@ -1967,21 +1955,21 @@
         <v>10</v>
       </c>
       <c r="P1" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="Q1" s="7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>34</v>
@@ -1989,139 +1977,73 @@
       <c r="E2" s="2"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>47</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>60</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="L2" s="1"/>
       <c r="M2" s="1" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
       <c r="P2" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>48</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
+      <c r="M3" s="1" t="s">
+        <v>111</v>
+      </c>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="1"/>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
-      <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
-      <c r="Q4" s="1"/>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
-      <c r="O5" s="1"/>
-      <c r="P5" s="1"/>
-      <c r="Q5" s="1"/>
+      <c r="P3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>51</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
@@ -2136,19 +2058,19 @@
           <x14:formula1>
             <xm:f>menus!$A$2:$A$16</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B5</xm:sqref>
+          <xm:sqref>B2:B3</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{FAA51CD0-43E0-A943-8055-0C5FB8D6C680}">
           <x14:formula1>
             <xm:f>menus!$E$2:$E$18</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C5</xm:sqref>
+          <xm:sqref>C2:C3</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{E5F9E90A-E21A-8A41-BB6A-B83D71712C77}">
           <x14:formula1>
             <xm:f>menus!$C$2:$C$8</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:E5</xm:sqref>
+          <xm:sqref>D2:E3</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2158,7 +2080,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD8FB4E8-B9B5-D24A-91D9-6FACBB875664}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2179,30 +2101,30 @@
         <v>7</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="G1" s="16" t="s">
         <v>10</v>
       </c>
       <c r="H1" s="16" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="I1" s="16" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="J1" s="16" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>23</v>
@@ -2218,31 +2140,55 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
+      <c r="A3" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
+      <c r="E3" s="1">
+        <v>100</v>
+      </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
+      <c r="I3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2" xr:uid="{50BE8285-A6CD-6B47-AB81-5D4070225B4F}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D3" xr:uid="{50BE8285-A6CD-6B47-AB81-5D4070225B4F}">
       <formula1>100</formula1>
       <formula2>20000</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2" xr:uid="{D1DB4BFA-83FC-0D44-A088-AFCB7C087252}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E3" xr:uid="{D1DB4BFA-83FC-0D44-A088-AFCB7C087252}">
       <formula1>10</formula1>
       <formula2>2000</formula2>
     </dataValidation>
@@ -2258,13 +2204,13 @@
           <x14:formula1>
             <xm:f>menus!$A$2:$A$16</xm:f>
           </x14:formula1>
-          <xm:sqref>B2</xm:sqref>
+          <xm:sqref>B2:B3</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8B6688A4-70D6-FC45-94AF-02BA5F718A94}">
           <x14:formula1>
             <xm:f>menus!$G$2:$G$5</xm:f>
           </x14:formula1>
-          <xm:sqref>C2</xm:sqref>
+          <xm:sqref>C2:C3</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2301,7 +2247,7 @@
         <v>37</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H1" s="12" t="s">
         <v>10</v>
@@ -2322,7 +2268,7 @@
         <v>39</v>
       </c>
       <c r="G2" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -2368,7 +2314,7 @@
         <v>37</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H5" s="12" t="s">
         <v>10</v>
@@ -2387,7 +2333,7 @@
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="G6" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -2454,7 +2400,7 @@
         <v>33</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="G2" t="s">
         <v>29</v>
@@ -2468,7 +2414,7 @@
         <v>34</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="G3" t="s">
         <v>30</v>
@@ -2479,10 +2425,10 @@
         <v>25</v>
       </c>
       <c r="C4" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="E4" s="11" t="s">
         <v>95</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>100</v>
       </c>
       <c r="G4" t="s">
         <v>31</v>
@@ -2490,13 +2436,13 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>35</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="G5" t="s">
         <v>32</v>
@@ -2504,109 +2450,109 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="17" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E17" s="11" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="18" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E18" s="11" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated mac version to 0.0.0.0.10
</commit_message>
<xml_diff>
--- a/examples/vpc.xlsx
+++ b/examples/vpc.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jww/Developer/python/terraformer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D834777-CACF-2748-8E4E-E366241AEAA3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D82BB93-7441-4149-B05A-D93A522A6A9A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38500" yWindow="-17420" windowWidth="25600" windowHeight="14680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="42020" yWindow="-15960" windowWidth="25600" windowHeight="14740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="vpc" sheetId="6" r:id="rId1"/>
     <sheet name="subnets" sheetId="26" r:id="rId2"/>
     <sheet name="instances" sheetId="27" r:id="rId3"/>
-    <sheet name="volumes" sheetId="49" r:id="rId4"/>
-    <sheet name="securitygroups" sheetId="4" r:id="rId5"/>
-    <sheet name="menus" sheetId="48" r:id="rId6"/>
+    <sheet name="networkinterfaces" sheetId="50" r:id="rId4"/>
+    <sheet name="volumes" sheetId="49" r:id="rId5"/>
+    <sheet name="securitygroups" sheetId="4" r:id="rId6"/>
+    <sheet name="menus" sheetId="48" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="122">
   <si>
     <t>public_gateway</t>
   </si>
@@ -167,18 +168,6 @@
     <t>classic_access</t>
   </si>
   <si>
-    <t>primary_nic_name</t>
-  </si>
-  <si>
-    <t>*primary_nic_subnet</t>
-  </si>
-  <si>
-    <t>primary_nic_security_groups</t>
-  </si>
-  <si>
-    <t>primary_nic_floating_ip</t>
-  </si>
-  <si>
     <t>vsi1nic0</t>
   </si>
   <si>
@@ -372,6 +361,48 @@
   </si>
   <si>
     <t>volume2</t>
+  </si>
+  <si>
+    <t>vsi1nic1</t>
+  </si>
+  <si>
+    <t>vsi2nic1</t>
+  </si>
+  <si>
+    <t>*instance</t>
+  </si>
+  <si>
+    <t>*subnet</t>
+  </si>
+  <si>
+    <t>security_groups</t>
+  </si>
+  <si>
+    <t>floating_ip</t>
+  </si>
+  <si>
+    <t>sg1,sg2</t>
+  </si>
+  <si>
+    <t>*primary_network_interface</t>
+  </si>
+  <si>
+    <t>Regions</t>
+  </si>
+  <si>
+    <t>Dallas</t>
+  </si>
+  <si>
+    <t>Frankfurt (Gen 1)</t>
+  </si>
+  <si>
+    <t>London (Gen 1)</t>
+  </si>
+  <si>
+    <t>Sydney (Gen 1)</t>
+  </si>
+  <si>
+    <t>Tokyo (Gen 1)</t>
   </si>
 </sst>
 </file>
@@ -540,7 +571,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="77">
+  <dxfs count="81">
     <dxf>
       <font>
         <b val="0"/>
@@ -810,6 +841,40 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1258,12 +1323,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{7215B7F5-B70C-6B42-84D7-6729B99B446D}" name="Table8" displayName="Table8" ref="A1:E2" totalsRowShown="0" headerRowDxfId="76" dataDxfId="75" tableBorderDxfId="74">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{7215B7F5-B70C-6B42-84D7-6729B99B446D}" name="Table8" displayName="Table8" ref="A1:E2" totalsRowShown="0" headerRowDxfId="80" dataDxfId="79" tableBorderDxfId="78">
   <autoFilter ref="A1:E2" xr:uid="{529F7172-ECCA-724F-9B2D-5A6C4B69CB3C}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{887BA8C8-9946-8A42-98DF-3633CAED0C28}" name="*name" dataDxfId="73"/>
-    <tableColumn id="5" xr3:uid="{5CEDAE6E-6D63-FE4C-B1E4-8EBD674619A5}" name="default_network_acl" dataDxfId="72"/>
-    <tableColumn id="2" xr3:uid="{A41B6291-1C2E-AB41-A22B-93622DC498B2}" name="classic_access" dataDxfId="71"/>
+    <tableColumn id="1" xr3:uid="{887BA8C8-9946-8A42-98DF-3633CAED0C28}" name="*name" dataDxfId="77"/>
+    <tableColumn id="5" xr3:uid="{5CEDAE6E-6D63-FE4C-B1E4-8EBD674619A5}" name="default_network_acl" dataDxfId="76"/>
+    <tableColumn id="2" xr3:uid="{A41B6291-1C2E-AB41-A22B-93622DC498B2}" name="classic_access" dataDxfId="75"/>
     <tableColumn id="4" xr3:uid="{9675255E-64F1-104E-BCF2-8AF88D430E4B}" name="resource_group"/>
     <tableColumn id="7" xr3:uid="{DF1FC027-D537-CB40-BAA8-AEAEE8D9E2C7}" name="tags"/>
   </tableColumns>
@@ -1272,8 +1337,22 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{97CF9BAD-1C51-BC47-AAC0-E356346EDEA4}" name="Table4" displayName="Table4" ref="A1:A16" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="A1:A16" xr:uid="{54D2B8C5-8B4B-6F48-ADDA-4AB0A92EEEC3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{5B120329-69CE-CF49-A040-777791D90941}" name="Table1820" displayName="Table1820" ref="A5:E7" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+  <autoFilter ref="A5:E7" xr:uid="{53EED686-95D2-F943-A81D-E27A130C6DAE}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{678669D2-0A26-204C-901F-75448A1A3221}" name="*name" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{B89C45C8-E3B8-F540-8BA1-08091D6ADB6B}" name="*direction" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{956D6B03-3EFB-C045-9DE1-C17FA24EE018}" name="*remote" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{723345A9-214D-9A4D-A11C-89900A05EB7C}" name="ip_version" dataDxfId="7"/>
+    <tableColumn id="10" xr3:uid="{8441EF0D-136D-E04F-8477-CE05C3A24F8E}" name="protocol" dataDxfId="6"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{97CF9BAD-1C51-BC47-AAC0-E356346EDEA4}" name="Table4" displayName="Table4" ref="C1:C16" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="C1:C16" xr:uid="{54D2B8C5-8B4B-6F48-ADDA-4AB0A92EEEC3}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{754440C3-162E-F748-AF02-EFAEF0209370}" name="Zones"/>
   </tableColumns>
@@ -1281,9 +1360,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{67A187D0-9C64-1D4D-B7B0-8EEEA34740FA}" name="Table9" displayName="Table9" ref="C1:C8" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
-  <autoFilter ref="C1:C8" xr:uid="{993A4077-8AAD-BA41-8838-666C07171DFB}"/>
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{67A187D0-9C64-1D4D-B7B0-8EEEA34740FA}" name="Table9" displayName="Table9" ref="E1:E8" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+  <autoFilter ref="E1:E8" xr:uid="{993A4077-8AAD-BA41-8838-666C07171DFB}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{B65CF56E-B04D-C14B-8A02-47B40A1CD02C}" name="Images" dataDxfId="2"/>
   </tableColumns>
@@ -1291,9 +1370,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{3386D107-B446-064C-A163-0DCBF02D35DE}" name="Table10" displayName="Table10" ref="E1:E18" totalsRowShown="0" dataDxfId="1">
-  <autoFilter ref="E1:E18" xr:uid="{3F6979D3-3BD1-E54D-A901-4B051BF78ECD}"/>
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{3386D107-B446-064C-A163-0DCBF02D35DE}" name="Table10" displayName="Table10" ref="G1:G18" totalsRowShown="0" dataDxfId="1">
+  <autoFilter ref="G1:G18" xr:uid="{3F6979D3-3BD1-E54D-A901-4B051BF78ECD}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{72946E87-41F5-D94C-9CC2-8311D0AD04FE}" name="Image Profiles" dataDxfId="0"/>
   </tableColumns>
@@ -1301,9 +1380,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{A9FFA773-1002-C74D-ACF1-C3340783F0C1}" name="Table12" displayName="Table12" ref="G1:G5" totalsRowShown="0">
-  <autoFilter ref="G1:G5" xr:uid="{CD560E84-DE1D-1B4A-9E17-CAB68CB40AB3}"/>
+<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{A9FFA773-1002-C74D-ACF1-C3340783F0C1}" name="Table12" displayName="Table12" ref="I1:I5" totalsRowShown="0">
+  <autoFilter ref="I1:I5" xr:uid="{CD560E84-DE1D-1B4A-9E17-CAB68CB40AB3}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{52D8B2A3-B9D4-284D-9EFF-740BEC22D9F1}" name="Volume Profiles"/>
   </tableColumns>
@@ -1311,66 +1390,87 @@
 </table>
 </file>
 
+<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{4EA443BC-F892-014C-AC8F-E553A221CAC5}" name="Table5" displayName="Table5" ref="A1:A6" totalsRowShown="0">
+  <autoFilter ref="A1:A6" xr:uid="{AECFE15C-8BD7-E24F-A643-2024F4043618}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{988DAC45-DC49-B940-9055-CFA8960B5FFF}" name="Regions"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CCDECB38-C0CC-2F45-942E-905874960FA1}" name="Table82" displayName="Table82" ref="G1:I2" totalsRowShown="0" headerRowDxfId="70" dataDxfId="69" tableBorderDxfId="68">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CCDECB38-C0CC-2F45-942E-905874960FA1}" name="Table82" displayName="Table82" ref="G1:I2" totalsRowShown="0" headerRowDxfId="74" dataDxfId="73" tableBorderDxfId="72">
   <autoFilter ref="G1:I2" xr:uid="{53320CC0-1502-AE46-960E-CBE997CAF081}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{1C4F7942-E10E-D542-96E0-A5F1B09D7653}" name="prefix_name" dataDxfId="67"/>
-    <tableColumn id="5" xr3:uid="{50A3D194-B2D5-7C45-82AC-A5F626E3A6D1}" name="zone" dataDxfId="66"/>
-    <tableColumn id="4" xr3:uid="{0FA22EA8-0E5A-2348-9F40-72141DF6B401}" name="cidr" dataDxfId="65"/>
+    <tableColumn id="1" xr3:uid="{1C4F7942-E10E-D542-96E0-A5F1B09D7653}" name="prefix_name" dataDxfId="71"/>
+    <tableColumn id="5" xr3:uid="{50A3D194-B2D5-7C45-82AC-A5F626E3A6D1}" name="zone" dataDxfId="70"/>
+    <tableColumn id="4" xr3:uid="{0FA22EA8-0E5A-2348-9F40-72141DF6B401}" name="cidr" dataDxfId="69"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{76790F31-1453-B641-9754-80A9D247EA0F}" name="Table6" displayName="Table6" ref="A1:J3" totalsRowShown="0" headerRowDxfId="64" dataDxfId="63">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{76790F31-1453-B641-9754-80A9D247EA0F}" name="Table6" displayName="Table6" ref="A1:J3" totalsRowShown="0" headerRowDxfId="68" dataDxfId="67">
   <autoFilter ref="A1:J3" xr:uid="{9725F296-5A96-A949-A782-B4A2B65596C4}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{1E9E58AF-C46F-2140-86A4-81396AD00F15}" name="*name" dataDxfId="62"/>
-    <tableColumn id="2" xr3:uid="{D989FA97-121E-ED4E-9CA5-25D303F38C24}" name="*zone" dataDxfId="61"/>
-    <tableColumn id="3" xr3:uid="{9DE77DE5-F660-7D4C-BC60-2B014D5E01EB}" name="ipv4_cidr_block" dataDxfId="60"/>
-    <tableColumn id="4" xr3:uid="{42D706D7-A721-6D49-8189-9A181B88E99F}" name="total_ipv4_address_count" dataDxfId="59"/>
-    <tableColumn id="5" xr3:uid="{215941D8-E315-5044-8E51-E2FEE9B95908}" name="ip_version" dataDxfId="58"/>
-    <tableColumn id="6" xr3:uid="{7CE7912A-5366-5A4D-9CAD-006BE9E02B39}" name="network_acl" dataDxfId="57"/>
-    <tableColumn id="7" xr3:uid="{87A1EA58-5C4B-0443-A650-07ABED9C6F31}" name="public_gateway" dataDxfId="56"/>
-    <tableColumn id="8" xr3:uid="{718DFD83-0842-7749-8498-7034DCF9F245}" name="create_timeout" dataDxfId="55"/>
-    <tableColumn id="9" xr3:uid="{6E310B89-982B-B743-8106-2EEBD001DB52}" name="update_timeout" dataDxfId="54"/>
-    <tableColumn id="10" xr3:uid="{16A0C085-1B24-8740-BCEF-FC5FBADEF6C0}" name="delete_timeout" dataDxfId="53"/>
+    <tableColumn id="1" xr3:uid="{1E9E58AF-C46F-2140-86A4-81396AD00F15}" name="*name" dataDxfId="66"/>
+    <tableColumn id="2" xr3:uid="{D989FA97-121E-ED4E-9CA5-25D303F38C24}" name="*zone" dataDxfId="65"/>
+    <tableColumn id="3" xr3:uid="{9DE77DE5-F660-7D4C-BC60-2B014D5E01EB}" name="ipv4_cidr_block" dataDxfId="64"/>
+    <tableColumn id="4" xr3:uid="{42D706D7-A721-6D49-8189-9A181B88E99F}" name="total_ipv4_address_count" dataDxfId="63"/>
+    <tableColumn id="5" xr3:uid="{215941D8-E315-5044-8E51-E2FEE9B95908}" name="ip_version" dataDxfId="62"/>
+    <tableColumn id="6" xr3:uid="{7CE7912A-5366-5A4D-9CAD-006BE9E02B39}" name="network_acl" dataDxfId="61"/>
+    <tableColumn id="7" xr3:uid="{87A1EA58-5C4B-0443-A650-07ABED9C6F31}" name="public_gateway" dataDxfId="60"/>
+    <tableColumn id="8" xr3:uid="{718DFD83-0842-7749-8498-7034DCF9F245}" name="create_timeout" dataDxfId="59"/>
+    <tableColumn id="9" xr3:uid="{6E310B89-982B-B743-8106-2EEBD001DB52}" name="update_timeout" dataDxfId="58"/>
+    <tableColumn id="10" xr3:uid="{16A0C085-1B24-8740-BCEF-FC5FBADEF6C0}" name="delete_timeout" dataDxfId="57"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{3F1E4605-7351-6A4A-9807-A10DCEAD79B7}" name="Table7" displayName="Table7" ref="A1:Q3" totalsRowShown="0" headerRowDxfId="52" dataDxfId="51">
-  <autoFilter ref="A1:Q3" xr:uid="{4F0FA061-E3B2-AB4E-A276-92C803DED60C}"/>
-  <tableColumns count="17">
-    <tableColumn id="1" xr3:uid="{B447E9AB-445F-0242-8396-EEAA92074797}" name="*name" dataDxfId="50"/>
-    <tableColumn id="2" xr3:uid="{E6843232-FC96-094F-809F-D9A2D9A3F5CB}" name="*zone" dataDxfId="49"/>
-    <tableColumn id="3" xr3:uid="{E7DB5053-DB66-CF46-AB33-5A411FF07264}" name="*profile" dataDxfId="48"/>
-    <tableColumn id="4" xr3:uid="{F65626CD-0D0E-D748-9934-00DB105BEEAC}" name="image" dataDxfId="47"/>
-    <tableColumn id="14" xr3:uid="{1A5FD37C-8F61-7B49-9DE5-C024F0CC91E5}" name="boot_volume_name" dataDxfId="46"/>
-    <tableColumn id="5" xr3:uid="{436C5517-AF19-1946-8EE7-03879E1F2944}" name="boot_volume_encryption" dataDxfId="45"/>
-    <tableColumn id="6" xr3:uid="{FFE24952-72F9-9D47-8A4B-2813BCCB260E}" name="*keys" dataDxfId="44"/>
-    <tableColumn id="9" xr3:uid="{A03604D8-6E33-4249-A9DE-BF8870E3D90B}" name="primary_nic_name" dataDxfId="43"/>
-    <tableColumn id="8" xr3:uid="{6BA991DA-676D-6A44-A3BB-F3F352C13290}" name="*primary_nic_subnet" dataDxfId="42"/>
-    <tableColumn id="11" xr3:uid="{22D3C3E8-9B81-9940-8B5C-FAB6544821B0}" name="primary_nic_security_groups" dataDxfId="41"/>
-    <tableColumn id="7" xr3:uid="{2843B70D-AC9D-5445-BD32-4CFA71397925}" name="primary_nic_floating_ip" dataDxfId="40"/>
-    <tableColumn id="10" xr3:uid="{438F95E2-E2D5-1E49-9852-4B915078693E}" name="network_interfaces" dataDxfId="39"/>
-    <tableColumn id="19" xr3:uid="{6293540A-4A05-0E4A-99ED-C75D3F46ECCF}" name="volumes" dataDxfId="38"/>
-    <tableColumn id="18" xr3:uid="{8C2D6431-BD15-6849-BBE1-C0EF1B26E51A}" name="user_data" dataDxfId="37"/>
-    <tableColumn id="17" xr3:uid="{8C7E9F80-830B-174D-9411-54916978023E}" name="resource_group" dataDxfId="36"/>
-    <tableColumn id="12" xr3:uid="{E2511928-0801-3546-B6BA-F9C8EF98BBC6}" name="create_timeout" dataDxfId="35"/>
-    <tableColumn id="13" xr3:uid="{F33A3F16-B62A-EC4B-BC5D-BAA56655B743}" name="delete_timeout" dataDxfId="34"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{3F1E4605-7351-6A4A-9807-A10DCEAD79B7}" name="Table7" displayName="Table7" ref="A1:N3" totalsRowShown="0" headerRowDxfId="56" dataDxfId="55">
+  <autoFilter ref="A1:N3" xr:uid="{4F0FA061-E3B2-AB4E-A276-92C803DED60C}"/>
+  <tableColumns count="14">
+    <tableColumn id="1" xr3:uid="{B447E9AB-445F-0242-8396-EEAA92074797}" name="*name" dataDxfId="54"/>
+    <tableColumn id="2" xr3:uid="{E6843232-FC96-094F-809F-D9A2D9A3F5CB}" name="*zone" dataDxfId="53"/>
+    <tableColumn id="3" xr3:uid="{E7DB5053-DB66-CF46-AB33-5A411FF07264}" name="*profile" dataDxfId="52"/>
+    <tableColumn id="4" xr3:uid="{F65626CD-0D0E-D748-9934-00DB105BEEAC}" name="image" dataDxfId="51"/>
+    <tableColumn id="14" xr3:uid="{1A5FD37C-8F61-7B49-9DE5-C024F0CC91E5}" name="boot_volume_name" dataDxfId="50"/>
+    <tableColumn id="5" xr3:uid="{436C5517-AF19-1946-8EE7-03879E1F2944}" name="boot_volume_encryption" dataDxfId="49"/>
+    <tableColumn id="6" xr3:uid="{FFE24952-72F9-9D47-8A4B-2813BCCB260E}" name="*keys" dataDxfId="48"/>
+    <tableColumn id="9" xr3:uid="{A03604D8-6E33-4249-A9DE-BF8870E3D90B}" name="*primary_network_interface" dataDxfId="47"/>
+    <tableColumn id="10" xr3:uid="{438F95E2-E2D5-1E49-9852-4B915078693E}" name="network_interfaces" dataDxfId="46"/>
+    <tableColumn id="19" xr3:uid="{6293540A-4A05-0E4A-99ED-C75D3F46ECCF}" name="volumes" dataDxfId="45"/>
+    <tableColumn id="18" xr3:uid="{8C2D6431-BD15-6849-BBE1-C0EF1B26E51A}" name="user_data" dataDxfId="44"/>
+    <tableColumn id="17" xr3:uid="{8C7E9F80-830B-174D-9411-54916978023E}" name="resource_group" dataDxfId="43"/>
+    <tableColumn id="12" xr3:uid="{E2511928-0801-3546-B6BA-F9C8EF98BBC6}" name="create_timeout" dataDxfId="42"/>
+    <tableColumn id="13" xr3:uid="{F33A3F16-B62A-EC4B-BC5D-BAA56655B743}" name="delete_timeout" dataDxfId="41"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C451A855-5250-674B-8039-E23EC3348E96}" name="Table11" displayName="Table11" ref="A1:J3" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
-  <autoFilter ref="A1:J3" xr:uid="{8CD156A6-A66F-1245-BCD2-9FAE26A0A77C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{81661C9C-F36C-2E41-BF2C-12573A860276}" name="Table75" displayName="Table75" ref="A1:E6" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39">
+  <autoFilter ref="A1:E6" xr:uid="{4F0FA061-E3B2-AB4E-A276-92C803DED60C}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{95E267F3-7620-8C4D-AFC7-4EB9DFAE946B}" name="*name" dataDxfId="38"/>
+    <tableColumn id="2" xr3:uid="{C13CAAAB-1F09-F442-B06D-36989DBA835A}" name="*instance" dataDxfId="37"/>
+    <tableColumn id="8" xr3:uid="{B55BB537-FA6A-D04D-99CC-63555EFADEB6}" name="*subnet" dataDxfId="36"/>
+    <tableColumn id="11" xr3:uid="{346BFF31-BC5B-C647-89BB-72AE7861274F}" name="security_groups" dataDxfId="35"/>
+    <tableColumn id="7" xr3:uid="{80D936B9-9EFA-6C4B-BF5E-9435B5B9B191}" name="floating_ip" dataDxfId="34"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C451A855-5250-674B-8039-E23EC3348E96}" name="Table11" displayName="Table11" ref="A1:J4" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
+  <autoFilter ref="A1:J4" xr:uid="{8CD156A6-A66F-1245-BCD2-9FAE26A0A77C}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{CDC18A34-D228-8E41-90CD-62AD9ACAF229}" name="*name" dataDxfId="31"/>
     <tableColumn id="2" xr3:uid="{480E110A-7DA0-1A46-B19A-DAB8291BA972}" name="*zone" dataDxfId="30"/>
@@ -1387,7 +1487,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{39E22F0D-DB3D-D64A-9C8B-1495DF50EA1D}" name="Table17" displayName="Table17" ref="G1:H2" totalsRowShown="0" headerRowDxfId="21">
   <autoFilter ref="G1:H2" xr:uid="{0A45E2CD-E273-B845-A6DC-901E2232E6DB}"/>
   <tableColumns count="2">
@@ -1398,7 +1498,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{D1930FB6-6EF2-5A4F-A1C5-080C14D74B21}" name="Table18" displayName="Table18" ref="A1:E3" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
   <autoFilter ref="A1:E3" xr:uid="{EF08DB4E-0002-F047-8599-404D4BBF8940}"/>
   <tableColumns count="5">
@@ -1412,26 +1512,12 @@
 </table>
 </file>
 
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{F21DE6D8-0A5C-3145-9A2B-E1F2A8034E09}" name="Table1719" displayName="Table1719" ref="G5:H6" totalsRowShown="0" headerRowDxfId="13">
   <autoFilter ref="G5:H6" xr:uid="{BA698B73-1CD9-D447-9915-33C13C4FA98F}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{3A290EFE-B770-574C-9295-B48616054705}" name="*group_name"/>
     <tableColumn id="2" xr3:uid="{00711262-18F5-6140-A437-4F27F0B7B26B}" name="resource_group"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{5B120329-69CE-CF49-A040-777791D90941}" name="Table1820" displayName="Table1820" ref="A5:E7" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
-  <autoFilter ref="A5:E7" xr:uid="{53EED686-95D2-F943-A81D-E27A130C6DAE}"/>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{678669D2-0A26-204C-901F-75448A1A3221}" name="*name" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{B89C45C8-E3B8-F540-8BA1-08091D6ADB6B}" name="*direction" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{956D6B03-3EFB-C045-9DE1-C17FA24EE018}" name="*remote" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{723345A9-214D-9A4D-A11C-89900A05EB7C}" name="ip_version" dataDxfId="7"/>
-    <tableColumn id="10" xr3:uid="{8441EF0D-136D-E04F-8477-CE05C3A24F8E}" name="protocol" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1729,21 +1815,21 @@
         <v>40</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B2" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="G2" s="14"/>
       <c r="H2" s="14"/>
@@ -1761,7 +1847,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{FAC53958-5205-4D43-A33A-8469C4A5BC91}">
           <x14:formula1>
-            <xm:f>menus!$A$2:$A$16</xm:f>
+            <xm:f>menus!$C$2:$C$16</xm:f>
           </x14:formula1>
           <xm:sqref>H2</xm:sqref>
         </x14:dataValidation>
@@ -1775,7 +1861,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58E633D9-8336-4776-A01F-1859C551A2C4}">
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1806,50 +1894,50 @@
         <v>0</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>24</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -1879,7 +1967,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C3DFCCB6-F847-9744-B65E-7CF60232C620}">
           <x14:formula1>
-            <xm:f>menus!$A$2:$A$16</xm:f>
+            <xm:f>menus!$C$2:$C$16</xm:f>
           </x14:formula1>
           <xm:sqref>B2:B3</xm:sqref>
         </x14:dataValidation>
@@ -1891,9 +1979,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69A31708-3A2C-4ADA-B3E5-8A1B18923F2A}">
-  <dimension ref="A1:Q3"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1901,14 +1991,14 @@
     <col min="4" max="4" width="32.83203125" customWidth="1"/>
     <col min="5" max="5" width="20.83203125" customWidth="1"/>
     <col min="6" max="6" width="22.83203125" customWidth="1"/>
-    <col min="7" max="8" width="20.83203125" customWidth="1"/>
-    <col min="9" max="10" width="25.83203125" customWidth="1"/>
+    <col min="7" max="7" width="20.83203125" customWidth="1"/>
+    <col min="8" max="10" width="25.83203125" customWidth="1"/>
     <col min="11" max="11" width="22.83203125" customWidth="1"/>
-    <col min="12" max="12" width="36.83203125" customWidth="1"/>
+    <col min="12" max="12" width="20.83203125" customWidth="1"/>
     <col min="13" max="15" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>6</v>
       </c>
@@ -1922,54 +2012,45 @@
         <v>2</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="G1" s="7" t="s">
         <v>8</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>44</v>
+        <v>115</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>36</v>
       </c>
       <c r="J1" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="N1" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="L1" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="M1" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="N1" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="O1" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="P1" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q1" s="7" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>34</v>
@@ -1977,42 +2058,35 @@
       <c r="E2" s="2"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>62</v>
+        <v>108</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>69</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="K2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>24</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>34</v>
@@ -2020,29 +2094,24 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>63</v>
+        <v>109</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>67</v>
+        <v>107</v>
       </c>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
-      <c r="P3" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -2056,19 +2125,19 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{88DE7120-2FCE-364C-A552-C3E89AB1A2C4}">
           <x14:formula1>
-            <xm:f>menus!$A$2:$A$16</xm:f>
+            <xm:f>menus!$C$2:$C$16</xm:f>
           </x14:formula1>
           <xm:sqref>B2:B3</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{FAA51CD0-43E0-A943-8055-0C5FB8D6C680}">
           <x14:formula1>
-            <xm:f>menus!$E$2:$E$18</xm:f>
+            <xm:f>menus!$G$2:$G$18</xm:f>
           </x14:formula1>
           <xm:sqref>C2:C3</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{E5F9E90A-E21A-8A41-BB6A-B83D71712C77}">
           <x14:formula1>
-            <xm:f>menus!$C$2:$C$8</xm:f>
+            <xm:f>menus!$E$2:$E$8</xm:f>
           </x14:formula1>
           <xm:sqref>D2:E3</xm:sqref>
         </x14:dataValidation>
@@ -2079,8 +2148,120 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FCD209A-28DD-7845-952F-4118CB029C17}">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="5" width="15.83203125" customWidth="1"/>
+    <col min="6" max="6" width="22.83203125" customWidth="1"/>
+    <col min="7" max="8" width="20.83203125" customWidth="1"/>
+    <col min="9" max="9" width="25.83203125" customWidth="1"/>
+    <col min="10" max="10" width="26.83203125" customWidth="1"/>
+    <col min="11" max="11" width="22.83203125" customWidth="1"/>
+    <col min="12" max="12" width="40.1640625" customWidth="1"/>
+    <col min="13" max="15" width="15.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E6" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD8FB4E8-B9B5-D24A-91D9-6FACBB875664}">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2101,30 +2282,30 @@
         <v>7</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="G1" s="16" t="s">
         <v>10</v>
       </c>
       <c r="H1" s="16" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="I1" s="16" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="J1" s="16" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>23</v>
@@ -2140,55 +2321,67 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>31</v>
-      </c>
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="1">
-        <v>100</v>
-      </c>
+      <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
-      <c r="I3" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>51</v>
-      </c>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
+      <c r="A4" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
+      <c r="E4" s="1">
+        <v>100</v>
+      </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
+      <c r="I4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D3" xr:uid="{50BE8285-A6CD-6B47-AB81-5D4070225B4F}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D4" xr:uid="{50BE8285-A6CD-6B47-AB81-5D4070225B4F}">
       <formula1>100</formula1>
       <formula2>20000</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E3" xr:uid="{D1DB4BFA-83FC-0D44-A088-AFCB7C087252}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E4" xr:uid="{D1DB4BFA-83FC-0D44-A088-AFCB7C087252}">
       <formula1>10</formula1>
       <formula2>2000</formula2>
     </dataValidation>
@@ -2202,15 +2395,15 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{14833FDB-C112-704E-9CEE-46E5E14AD65D}">
           <x14:formula1>
-            <xm:f>menus!$A$2:$A$16</xm:f>
+            <xm:f>menus!$C$2:$C$16</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B3</xm:sqref>
+          <xm:sqref>B2:B4</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8B6688A4-70D6-FC45-94AF-02BA5F718A94}">
           <x14:formula1>
-            <xm:f>menus!$G$2:$G$5</xm:f>
+            <xm:f>menus!$I$2:$I$5</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C3</xm:sqref>
+          <xm:sqref>C2:C4</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2218,7 +2411,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I7"/>
   <sheetViews>
@@ -2247,7 +2440,7 @@
         <v>37</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="H1" s="12" t="s">
         <v>10</v>
@@ -2268,7 +2461,7 @@
         <v>39</v>
       </c>
       <c r="G2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -2314,7 +2507,7 @@
         <v>37</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="H5" s="12" t="s">
         <v>10</v>
@@ -2333,7 +2526,7 @@
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="G6" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -2361,9 +2554,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A27DA9FB-C6DE-DD43-83A1-C14B1BF5FE4D}">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2371,197 +2564,218 @@
   <cols>
     <col min="1" max="1" width="15.83203125" customWidth="1"/>
     <col min="2" max="2" width="1.83203125" customWidth="1"/>
-    <col min="3" max="3" width="63.83203125" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" customWidth="1"/>
     <col min="4" max="4" width="1.83203125" customWidth="1"/>
-    <col min="5" max="5" width="44.83203125" customWidth="1"/>
+    <col min="5" max="5" width="63.83203125" customWidth="1"/>
     <col min="6" max="6" width="1.83203125" customWidth="1"/>
-    <col min="7" max="7" width="15.83203125" customWidth="1"/>
+    <col min="7" max="7" width="44.83203125" customWidth="1"/>
+    <col min="8" max="8" width="1.83203125" customWidth="1"/>
+    <col min="9" max="9" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>27</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C2" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="E2" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="G2" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="I2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="I3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="I4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>120</v>
+      </c>
+      <c r="C5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="I5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>121</v>
+      </c>
+      <c r="C6" t="s">
+        <v>75</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="G7" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="G2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="G3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="E4" s="11" t="s">
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C8" t="s">
+        <v>77</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C9" t="s">
+        <v>78</v>
+      </c>
+      <c r="G9" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="G4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="E5" s="11" t="s">
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C10" t="s">
+        <v>79</v>
+      </c>
+      <c r="G10" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="G5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>79</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="E6" s="11" t="s">
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C11" t="s">
+        <v>80</v>
+      </c>
+      <c r="G11" s="11" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>80</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="E7" s="11" t="s">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C12" t="s">
+        <v>81</v>
+      </c>
+      <c r="G12" s="11" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>81</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C13" t="s">
         <v>82</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="G13" s="11" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C14" t="s">
         <v>83</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="G14" s="11" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C15" t="s">
         <v>84</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="G15" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C16" t="s">
         <v>85</v>
       </c>
-      <c r="E12" s="11" t="s">
+      <c r="G16" s="11" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>86</v>
-      </c>
-      <c r="E13" s="11" t="s">
+    <row r="17" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G17" s="11" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>87</v>
-      </c>
-      <c r="E14" s="11" t="s">
+    <row r="18" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G18" s="11" t="s">
         <v>104</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>88</v>
-      </c>
-      <c r="E15" s="11" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>89</v>
-      </c>
-      <c r="E16" s="11" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E17" s="11" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="18" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E18" s="11" t="s">
-        <v>108</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="4">
+  <tableParts count="5">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated mac version to 0.0.0.0.15
</commit_message>
<xml_diff>
--- a/examples/vpc.xlsx
+++ b/examples/vpc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jww/Developer/python/terraformer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AAD9C93-B09E-5E45-B225-60AB7436881E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F149B92-FADB-414C-98C3-67AA253559F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2840" yWindow="460" windowWidth="25600" windowHeight="14700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="vpcheaders" sheetId="6" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="instances" sheetId="27" r:id="rId4"/>
     <sheet name="networkinterfaces" sheetId="50" r:id="rId5"/>
     <sheet name="volumes" sheetId="49" r:id="rId6"/>
-    <sheet name="menus" sheetId="48" r:id="rId7"/>
+    <sheet name="images" sheetId="52" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="67">
   <si>
     <t>public_gateway</t>
   </si>
@@ -75,48 +75,12 @@
     <t>network_acl</t>
   </si>
   <si>
-    <t>Zones</t>
-  </si>
-  <si>
     <t>Dallas 1</t>
   </si>
   <si>
     <t>Dallas 2</t>
   </si>
   <si>
-    <t>Dallas 3</t>
-  </si>
-  <si>
-    <t>Images</t>
-  </si>
-  <si>
-    <t>Image Profiles</t>
-  </si>
-  <si>
-    <t>Volume Profiles</t>
-  </si>
-  <si>
-    <t>3 IOPS/GB</t>
-  </si>
-  <si>
-    <t>5 IOPS/GB</t>
-  </si>
-  <si>
-    <t>10 IOPS/GB</t>
-  </si>
-  <si>
-    <t>Custom</t>
-  </si>
-  <si>
-    <t>CentOS 7.x - Minimal Install</t>
-  </si>
-  <si>
-    <t>Debian GNU/Linux 9.x - Minimal Install</t>
-  </si>
-  <si>
-    <t>Ubuntu Linux 18.04 LTS - Minimal Install</t>
-  </si>
-  <si>
     <t>network_interfaces</t>
   </si>
   <si>
@@ -201,105 +165,6 @@
     <t>volume1</t>
   </si>
   <si>
-    <t>Frankfurt 1 (Gen 1)</t>
-  </si>
-  <si>
-    <t>Frankfurt 2 (Gen 1)</t>
-  </si>
-  <si>
-    <t>Frankfurt 3 (Gen 1)</t>
-  </si>
-  <si>
-    <t>London 1 (Gen 1)</t>
-  </si>
-  <si>
-    <t>London 2 (Gen 1)</t>
-  </si>
-  <si>
-    <t>London 3 (Gen 1)</t>
-  </si>
-  <si>
-    <t>Sydney 1 (Gen 1)</t>
-  </si>
-  <si>
-    <t>Sydney 2 (Gen 1)</t>
-  </si>
-  <si>
-    <t>Sydney 3 (Gen 1)</t>
-  </si>
-  <si>
-    <t>Tokyo 1 (Gen 1)</t>
-  </si>
-  <si>
-    <t>Tokyo 2 (Gen 1)</t>
-  </si>
-  <si>
-    <t>Tokyo 3 (Gen 1)</t>
-  </si>
-  <si>
-    <t>Red Hat Enterprise Linux 7.x - Minimal Install (Gen 1)</t>
-  </si>
-  <si>
-    <t>Windows Server 2012 Standard Edition (Gen 1)</t>
-  </si>
-  <si>
-    <t>Windows Server 2012 R2 Standard Edition (Gen 1)</t>
-  </si>
-  <si>
-    <t>Windows Server 2016 Standard Edition (Gen 1)</t>
-  </si>
-  <si>
-    <t>Balanced 2 vCPUs x 8GB RAM</t>
-  </si>
-  <si>
-    <t>Balanced 8 vCPUs x 32GB RAM</t>
-  </si>
-  <si>
-    <t>Balanced 16 vCPUs x 64GB RAM</t>
-  </si>
-  <si>
-    <t>Balanced 32 vCPUs x 128GB RAM</t>
-  </si>
-  <si>
-    <t>Balanced 48 vCPUs x 192GB RAM</t>
-  </si>
-  <si>
-    <t>Compute 2 vCPUs x 4GB RAM</t>
-  </si>
-  <si>
-    <t>Compute 4 vCPUs x 8GB RAM</t>
-  </si>
-  <si>
-    <t>Compute 8 vCPUs x 16GB RAM</t>
-  </si>
-  <si>
-    <t>Compute 16 vCPUs x 32GB RAM</t>
-  </si>
-  <si>
-    <t>Compute 32 vCPUs x 64GB RAM</t>
-  </si>
-  <si>
-    <t>Memory 2 vCPUs x 16GB RAM</t>
-  </si>
-  <si>
-    <t>Memory 4 vCPUs x 32GB RAM</t>
-  </si>
-  <si>
-    <t>Memory 8 vCPUs x 64GB RAM</t>
-  </si>
-  <si>
-    <t>Memory 16 vCPUs x 128GB RAM</t>
-  </si>
-  <si>
-    <t>Memory 32 vCPUs x 256GB RAM</t>
-  </si>
-  <si>
-    <t>Balanced 4 vCPUs x 16GB RAM (Gen 1)</t>
-  </si>
-  <si>
-    <t>Balanced 62 vCPUs x 248GB RAM (Gen 1)</t>
-  </si>
-  <si>
     <t>volume2</t>
   </si>
   <si>
@@ -327,24 +192,6 @@
     <t>*primary_network_interface</t>
   </si>
   <si>
-    <t>Regions</t>
-  </si>
-  <si>
-    <t>Dallas</t>
-  </si>
-  <si>
-    <t>Frankfurt (Gen 1)</t>
-  </si>
-  <si>
-    <t>London (Gen 1)</t>
-  </si>
-  <si>
-    <t>Sydney (Gen 1)</t>
-  </si>
-  <si>
-    <t>Tokyo (Gen 1)</t>
-  </si>
-  <si>
     <t>vsi1nic0primary</t>
   </si>
   <si>
@@ -376,13 +223,28 @@
   </si>
   <si>
     <t>10.240.64.0/18</t>
+  </si>
+  <si>
+    <t>bx2-8x32</t>
+  </si>
+  <si>
+    <t>ibm-debian9-amd64</t>
+  </si>
+  <si>
+    <t>10iops-tier</t>
+  </si>
+  <si>
+    <t>*href</t>
+  </si>
+  <si>
+    <t>*operating_system</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -414,19 +276,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Menlo"/>
+      <sz val="8"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Menlo"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="8"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -502,10 +360,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -521,89 +380,31 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="67">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Menlo"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Menlo"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Menlo"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Menlo"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
+  <dxfs count="66">
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -612,14 +413,7 @@
           <bgColor theme="4"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1158,13 +952,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{7215B7F5-B70C-6B42-84D7-6729B99B446D}" name="Table8" displayName="Table8" ref="A1:F3" totalsRowShown="0" headerRowDxfId="66" dataDxfId="65" tableBorderDxfId="64">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{7215B7F5-B70C-6B42-84D7-6729B99B446D}" name="Table8" displayName="Table8" ref="A1:F3" totalsRowShown="0" headerRowDxfId="65" dataDxfId="64" tableBorderDxfId="63">
   <autoFilter ref="A1:F3" xr:uid="{529F7172-ECCA-724F-9B2D-5A6C4B69CB3C}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{887BA8C8-9946-8A42-98DF-3633CAED0C28}" name="*name" dataDxfId="63"/>
-    <tableColumn id="5" xr3:uid="{5CEDAE6E-6D63-FE4C-B1E4-8EBD674619A5}" name="default_network_acl" dataDxfId="62"/>
+    <tableColumn id="1" xr3:uid="{887BA8C8-9946-8A42-98DF-3633CAED0C28}" name="*name" dataDxfId="62"/>
+    <tableColumn id="5" xr3:uid="{5CEDAE6E-6D63-FE4C-B1E4-8EBD674619A5}" name="default_network_acl" dataDxfId="61"/>
     <tableColumn id="3" xr3:uid="{D2048242-D53A-2A48-924A-8019052FD266}" name="address_prefix_management"/>
-    <tableColumn id="2" xr3:uid="{A41B6291-1C2E-AB41-A22B-93622DC498B2}" name="classic_access" dataDxfId="61"/>
+    <tableColumn id="2" xr3:uid="{A41B6291-1C2E-AB41-A22B-93622DC498B2}" name="classic_access" dataDxfId="60"/>
     <tableColumn id="4" xr3:uid="{9675255E-64F1-104E-BCF2-8AF88D430E4B}" name="resource_group"/>
     <tableColumn id="7" xr3:uid="{DF1FC027-D537-CB40-BAA8-AEAEE8D9E2C7}" name="tags"/>
   </tableColumns>
@@ -1172,143 +966,105 @@
 </table>
 </file>
 
-<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{A9FFA773-1002-C74D-ACF1-C3340783F0C1}" name="Table12" displayName="Table12" ref="I1:I5" totalsRowShown="0">
-  <autoFilter ref="I1:I5" xr:uid="{CD560E84-DE1D-1B4A-9E17-CAB68CB40AB3}"/>
-  <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{52D8B2A3-B9D4-284D-9EFF-740BEC22D9F1}" name="Volume Profiles"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{4EA443BC-F892-014C-AC8F-E553A221CAC5}" name="Table5" displayName="Table5" ref="A1:A6" totalsRowShown="0">
-  <autoFilter ref="A1:A6" xr:uid="{AECFE15C-8BD7-E24F-A643-2024F4043618}"/>
-  <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{988DAC45-DC49-B940-9055-CFA8960B5FFF}" name="Regions"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{80420FF8-12AA-D148-A5E9-F305380E9AC4}" name="Table82" displayName="Table82" ref="A1:D3" totalsRowShown="0" headerRowDxfId="60" dataDxfId="59" tableBorderDxfId="58">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{80420FF8-12AA-D148-A5E9-F305380E9AC4}" name="Table82" displayName="Table82" ref="A1:D3" totalsRowShown="0" headerRowDxfId="59" dataDxfId="58" tableBorderDxfId="57">
   <autoFilter ref="A1:D3" xr:uid="{9C9BAFE8-9631-CE45-93B1-83DB9C4014D5}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{C6C9ADE6-AC77-4944-9C6C-9D136392888D}" name="*name" dataDxfId="57"/>
-    <tableColumn id="5" xr3:uid="{0731D78F-C6D2-8948-BD0A-FB61D3B47F6C}" name="*vpc" dataDxfId="56"/>
+    <tableColumn id="1" xr3:uid="{C6C9ADE6-AC77-4944-9C6C-9D136392888D}" name="*name" dataDxfId="56"/>
+    <tableColumn id="5" xr3:uid="{0731D78F-C6D2-8948-BD0A-FB61D3B47F6C}" name="*vpc" dataDxfId="55"/>
     <tableColumn id="3" xr3:uid="{A408C4C2-23CE-B443-BA1D-7440072D5651}" name="*zone"/>
-    <tableColumn id="2" xr3:uid="{F0825E63-100E-584C-B142-E4481E9F997C}" name="*cidr" dataDxfId="55"/>
+    <tableColumn id="2" xr3:uid="{F0825E63-100E-584C-B142-E4481E9F997C}" name="*cidr" dataDxfId="54"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{76790F31-1453-B641-9754-80A9D247EA0F}" name="Table6" displayName="Table6" ref="A1:K3" totalsRowShown="0" headerRowDxfId="54" dataDxfId="53">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{76790F31-1453-B641-9754-80A9D247EA0F}" name="Table6" displayName="Table6" ref="A1:K3" totalsRowShown="0" headerRowDxfId="53" dataDxfId="52">
   <autoFilter ref="A1:K3" xr:uid="{9725F296-5A96-A949-A782-B4A2B65596C4}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{1E9E58AF-C46F-2140-86A4-81396AD00F15}" name="*name" dataDxfId="52"/>
-    <tableColumn id="11" xr3:uid="{9C2673D8-AB9A-9645-A3ED-D9B779022434}" name="*vpc" dataDxfId="51"/>
-    <tableColumn id="2" xr3:uid="{D989FA97-121E-ED4E-9CA5-25D303F38C24}" name="*zone" dataDxfId="50"/>
-    <tableColumn id="3" xr3:uid="{9DE77DE5-F660-7D4C-BC60-2B014D5E01EB}" name="ipv4_cidr_block" dataDxfId="49"/>
-    <tableColumn id="4" xr3:uid="{42D706D7-A721-6D49-8189-9A181B88E99F}" name="total_ipv4_address_count" dataDxfId="48"/>
-    <tableColumn id="5" xr3:uid="{215941D8-E315-5044-8E51-E2FEE9B95908}" name="ip_version" dataDxfId="47"/>
-    <tableColumn id="6" xr3:uid="{7CE7912A-5366-5A4D-9CAD-006BE9E02B39}" name="network_acl" dataDxfId="46"/>
-    <tableColumn id="7" xr3:uid="{87A1EA58-5C4B-0443-A650-07ABED9C6F31}" name="public_gateway" dataDxfId="45"/>
-    <tableColumn id="8" xr3:uid="{718DFD83-0842-7749-8498-7034DCF9F245}" name="create_timeout" dataDxfId="44"/>
-    <tableColumn id="9" xr3:uid="{6E310B89-982B-B743-8106-2EEBD001DB52}" name="update_timeout" dataDxfId="43"/>
-    <tableColumn id="10" xr3:uid="{16A0C085-1B24-8740-BCEF-FC5FBADEF6C0}" name="delete_timeout" dataDxfId="42"/>
+    <tableColumn id="1" xr3:uid="{1E9E58AF-C46F-2140-86A4-81396AD00F15}" name="*name" dataDxfId="51"/>
+    <tableColumn id="11" xr3:uid="{9C2673D8-AB9A-9645-A3ED-D9B779022434}" name="*vpc" dataDxfId="50"/>
+    <tableColumn id="2" xr3:uid="{D989FA97-121E-ED4E-9CA5-25D303F38C24}" name="*zone" dataDxfId="49"/>
+    <tableColumn id="3" xr3:uid="{9DE77DE5-F660-7D4C-BC60-2B014D5E01EB}" name="ipv4_cidr_block" dataDxfId="48"/>
+    <tableColumn id="4" xr3:uid="{42D706D7-A721-6D49-8189-9A181B88E99F}" name="total_ipv4_address_count" dataDxfId="47"/>
+    <tableColumn id="5" xr3:uid="{215941D8-E315-5044-8E51-E2FEE9B95908}" name="ip_version" dataDxfId="46"/>
+    <tableColumn id="6" xr3:uid="{7CE7912A-5366-5A4D-9CAD-006BE9E02B39}" name="network_acl" dataDxfId="45"/>
+    <tableColumn id="7" xr3:uid="{87A1EA58-5C4B-0443-A650-07ABED9C6F31}" name="public_gateway" dataDxfId="44"/>
+    <tableColumn id="8" xr3:uid="{718DFD83-0842-7749-8498-7034DCF9F245}" name="create_timeout" dataDxfId="43"/>
+    <tableColumn id="9" xr3:uid="{6E310B89-982B-B743-8106-2EEBD001DB52}" name="update_timeout" dataDxfId="42"/>
+    <tableColumn id="10" xr3:uid="{16A0C085-1B24-8740-BCEF-FC5FBADEF6C0}" name="delete_timeout" dataDxfId="41"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{3F1E4605-7351-6A4A-9807-A10DCEAD79B7}" name="Table7" displayName="Table7" ref="A1:O3" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{3F1E4605-7351-6A4A-9807-A10DCEAD79B7}" name="Table7" displayName="Table7" ref="A1:O3" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39">
   <autoFilter ref="A1:O3" xr:uid="{4F0FA061-E3B2-AB4E-A276-92C803DED60C}"/>
   <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{B447E9AB-445F-0242-8396-EEAA92074797}" name="*name" dataDxfId="39"/>
-    <tableColumn id="7" xr3:uid="{AECA3B2B-972B-2947-B76F-3FE48277F64A}" name="*vpc" dataDxfId="38"/>
-    <tableColumn id="2" xr3:uid="{E6843232-FC96-094F-809F-D9A2D9A3F5CB}" name="*zone" dataDxfId="37"/>
-    <tableColumn id="3" xr3:uid="{E7DB5053-DB66-CF46-AB33-5A411FF07264}" name="*profile" dataDxfId="36"/>
-    <tableColumn id="4" xr3:uid="{F65626CD-0D0E-D748-9934-00DB105BEEAC}" name="*image" dataDxfId="35"/>
-    <tableColumn id="14" xr3:uid="{1A5FD37C-8F61-7B49-9DE5-C024F0CC91E5}" name="boot_volume_name" dataDxfId="34"/>
-    <tableColumn id="5" xr3:uid="{436C5517-AF19-1946-8EE7-03879E1F2944}" name="boot_volume_encryption" dataDxfId="33"/>
-    <tableColumn id="6" xr3:uid="{FFE24952-72F9-9D47-8A4B-2813BCCB260E}" name="*keys" dataDxfId="32"/>
-    <tableColumn id="9" xr3:uid="{A03604D8-6E33-4249-A9DE-BF8870E3D90B}" name="*primary_network_interface" dataDxfId="31"/>
-    <tableColumn id="10" xr3:uid="{438F95E2-E2D5-1E49-9852-4B915078693E}" name="network_interfaces" dataDxfId="30"/>
-    <tableColumn id="19" xr3:uid="{6293540A-4A05-0E4A-99ED-C75D3F46ECCF}" name="volumes" dataDxfId="29"/>
-    <tableColumn id="18" xr3:uid="{8C2D6431-BD15-6849-BBE1-C0EF1B26E51A}" name="user_data" dataDxfId="28"/>
-    <tableColumn id="17" xr3:uid="{8C7E9F80-830B-174D-9411-54916978023E}" name="resource_group" dataDxfId="27"/>
-    <tableColumn id="12" xr3:uid="{E2511928-0801-3546-B6BA-F9C8EF98BBC6}" name="create_timeout" dataDxfId="26"/>
-    <tableColumn id="13" xr3:uid="{F33A3F16-B62A-EC4B-BC5D-BAA56655B743}" name="delete_timeout" dataDxfId="25"/>
+    <tableColumn id="1" xr3:uid="{B447E9AB-445F-0242-8396-EEAA92074797}" name="*name" dataDxfId="38"/>
+    <tableColumn id="7" xr3:uid="{AECA3B2B-972B-2947-B76F-3FE48277F64A}" name="*vpc" dataDxfId="37"/>
+    <tableColumn id="2" xr3:uid="{E6843232-FC96-094F-809F-D9A2D9A3F5CB}" name="*zone" dataDxfId="36"/>
+    <tableColumn id="3" xr3:uid="{E7DB5053-DB66-CF46-AB33-5A411FF07264}" name="*profile" dataDxfId="35"/>
+    <tableColumn id="4" xr3:uid="{F65626CD-0D0E-D748-9934-00DB105BEEAC}" name="*image" dataDxfId="34"/>
+    <tableColumn id="14" xr3:uid="{1A5FD37C-8F61-7B49-9DE5-C024F0CC91E5}" name="boot_volume_name" dataDxfId="33"/>
+    <tableColumn id="5" xr3:uid="{436C5517-AF19-1946-8EE7-03879E1F2944}" name="boot_volume_encryption" dataDxfId="32"/>
+    <tableColumn id="6" xr3:uid="{FFE24952-72F9-9D47-8A4B-2813BCCB260E}" name="*keys" dataDxfId="31"/>
+    <tableColumn id="9" xr3:uid="{A03604D8-6E33-4249-A9DE-BF8870E3D90B}" name="*primary_network_interface" dataDxfId="30"/>
+    <tableColumn id="10" xr3:uid="{438F95E2-E2D5-1E49-9852-4B915078693E}" name="network_interfaces" dataDxfId="29"/>
+    <tableColumn id="19" xr3:uid="{6293540A-4A05-0E4A-99ED-C75D3F46ECCF}" name="volumes" dataDxfId="28"/>
+    <tableColumn id="18" xr3:uid="{8C2D6431-BD15-6849-BBE1-C0EF1B26E51A}" name="user_data" dataDxfId="27"/>
+    <tableColumn id="17" xr3:uid="{8C7E9F80-830B-174D-9411-54916978023E}" name="resource_group" dataDxfId="26"/>
+    <tableColumn id="12" xr3:uid="{E2511928-0801-3546-B6BA-F9C8EF98BBC6}" name="create_timeout" dataDxfId="25"/>
+    <tableColumn id="13" xr3:uid="{F33A3F16-B62A-EC4B-BC5D-BAA56655B743}" name="delete_timeout" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{81661C9C-F36C-2E41-BF2C-12573A860276}" name="Table75" displayName="Table75" ref="A1:E5" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{81661C9C-F36C-2E41-BF2C-12573A860276}" name="Table75" displayName="Table75" ref="A1:E5" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
   <autoFilter ref="A1:E5" xr:uid="{4F0FA061-E3B2-AB4E-A276-92C803DED60C}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{95E267F3-7620-8C4D-AFC7-4EB9DFAE946B}" name="*name" dataDxfId="22"/>
-    <tableColumn id="2" xr3:uid="{C13CAAAB-1F09-F442-B06D-36989DBA835A}" name="*instance" dataDxfId="21"/>
-    <tableColumn id="8" xr3:uid="{B55BB537-FA6A-D04D-99CC-63555EFADEB6}" name="*subnet" dataDxfId="20"/>
-    <tableColumn id="11" xr3:uid="{346BFF31-BC5B-C647-89BB-72AE7861274F}" name="security_groups" dataDxfId="19"/>
-    <tableColumn id="7" xr3:uid="{80D936B9-9EFA-6C4B-BF5E-9435B5B9B191}" name="floating_ip" dataDxfId="18"/>
+    <tableColumn id="1" xr3:uid="{95E267F3-7620-8C4D-AFC7-4EB9DFAE946B}" name="*name" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{C13CAAAB-1F09-F442-B06D-36989DBA835A}" name="*instance" dataDxfId="20"/>
+    <tableColumn id="8" xr3:uid="{B55BB537-FA6A-D04D-99CC-63555EFADEB6}" name="*subnet" dataDxfId="19"/>
+    <tableColumn id="11" xr3:uid="{346BFF31-BC5B-C647-89BB-72AE7861274F}" name="security_groups" dataDxfId="18"/>
+    <tableColumn id="7" xr3:uid="{80D936B9-9EFA-6C4B-BF5E-9435B5B9B191}" name="floating_ip" dataDxfId="17"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C451A855-5250-674B-8039-E23EC3348E96}" name="Table11" displayName="Table11" ref="A1:J3" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C451A855-5250-674B-8039-E23EC3348E96}" name="Table11" displayName="Table11" ref="A1:J3" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
   <autoFilter ref="A1:J3" xr:uid="{8CD156A6-A66F-1245-BCD2-9FAE26A0A77C}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{CDC18A34-D228-8E41-90CD-62AD9ACAF229}" name="*name" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{480E110A-7DA0-1A46-B19A-DAB8291BA972}" name="*zone" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{1B453B9B-A3A5-5948-96F3-62C87F788C3A}" name="*profile" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{6CC60290-7B72-D343-A43F-F0F762500CF4}" name="iops" dataDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{45C880C0-FF4F-2F4A-919A-124DB93E5010}" name="capacity" dataDxfId="11"/>
-    <tableColumn id="6" xr3:uid="{787D8375-0B24-5F42-A273-3093BD8B60EC}" name="encryption_key" dataDxfId="10"/>
-    <tableColumn id="7" xr3:uid="{392944E6-6831-6F41-86DE-438B3577B0C6}" name="resource_group" dataDxfId="9"/>
-    <tableColumn id="8" xr3:uid="{2D73C361-1CE6-FF4D-BC45-651F77AC5BE1}" name="resource_controller_url" dataDxfId="8"/>
-    <tableColumn id="9" xr3:uid="{DC38DEC2-7381-DD45-A09D-F3050D08CA1E}" name="create_timeout" dataDxfId="7"/>
-    <tableColumn id="10" xr3:uid="{63225B45-4949-7A45-9F18-531EB8888D63}" name="delete_timeout" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{CDC18A34-D228-8E41-90CD-62AD9ACAF229}" name="*name" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{480E110A-7DA0-1A46-B19A-DAB8291BA972}" name="*zone" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{1B453B9B-A3A5-5948-96F3-62C87F788C3A}" name="*profile" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{6CC60290-7B72-D343-A43F-F0F762500CF4}" name="iops" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{45C880C0-FF4F-2F4A-919A-124DB93E5010}" name="capacity" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{787D8375-0B24-5F42-A273-3093BD8B60EC}" name="encryption_key" dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{392944E6-6831-6F41-86DE-438B3577B0C6}" name="resource_group" dataDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{2D73C361-1CE6-FF4D-BC45-651F77AC5BE1}" name="resource_controller_url" dataDxfId="7"/>
+    <tableColumn id="9" xr3:uid="{DC38DEC2-7381-DD45-A09D-F3050D08CA1E}" name="create_timeout" dataDxfId="6"/>
+    <tableColumn id="10" xr3:uid="{63225B45-4949-7A45-9F18-531EB8888D63}" name="delete_timeout" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{97CF9BAD-1C51-BC47-AAC0-E356346EDEA4}" name="Table4" displayName="Table4" ref="C1:C16" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="C1:C16" xr:uid="{54D2B8C5-8B4B-6F48-ADDA-4AB0A92EEEC3}"/>
-  <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{754440C3-162E-F748-AF02-EFAEF0209370}" name="Zones"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5CC6AE3F-9734-ED45-8903-103E4A3651C5}" name="Table323" displayName="Table323" ref="A1:C3" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+  <autoFilter ref="A1:C3" xr:uid="{DC08D300-10E5-4A45-A724-480E99186CDC}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{9D2269D2-DAC7-7A44-AA65-217A6B5A9326}" name="*name" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{AA9DBEBB-EC6B-E848-9DA7-CEA5574D32E3}" name="*href" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{4531D242-4648-604D-A4F0-6C45B93511A5}" name="*operating_system" dataDxfId="0"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{67A187D0-9C64-1D4D-B7B0-8EEEA34740FA}" name="Table9" displayName="Table9" ref="E1:E8" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
-  <autoFilter ref="E1:E8" xr:uid="{993A4077-8AAD-BA41-8838-666C07171DFB}"/>
-  <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{B65CF56E-B04D-C14B-8A02-47B40A1CD02C}" name="Images" dataDxfId="2"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{3386D107-B446-064C-A163-0DCBF02D35DE}" name="Table10" displayName="Table10" ref="G1:G18" totalsRowShown="0" dataDxfId="1">
-  <autoFilter ref="G1:G18" xr:uid="{3F6979D3-3BD1-E54D-A901-4B051BF78ECD}"/>
-  <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{72946E87-41F5-D94C-9CC2-8311D0AD04FE}" name="Image Profiles" dataDxfId="0"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -1592,36 +1348,36 @@
         <v>4</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>107</v>
+        <v>56</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="11" t="s">
-        <v>27</v>
+      <c r="F1" s="9" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
-        <v>108</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="12"/>
-      <c r="B3" s="12"/>
-      <c r="D3" s="12"/>
+      <c r="A3" s="10"/>
+      <c r="B3" s="10"/>
+      <c r="D3" s="10"/>
     </row>
   </sheetData>
   <dataConsolidate/>
@@ -1648,41 +1404,41 @@
         <v>4</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>104</v>
+        <v>53</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>3</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>105</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>109</v>
+        <v>58</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" t="s">
         <v>13</v>
       </c>
-      <c r="D2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="12" t="s">
-        <v>110</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>112</v>
+      <c r="D3" s="10" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1691,18 +1447,6 @@
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C99D23D2-AA69-9C46-A58D-A4A1D68C786E}">
-          <x14:formula1>
-            <xm:f>menus!$C$2:$C$16</xm:f>
-          </x14:formula1>
-          <xm:sqref>C2:C3</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -1723,7 +1467,7 @@
         <v>4</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>104</v>
+        <v>53</v>
       </c>
       <c r="C1" t="s">
         <v>3</v>
@@ -1744,56 +1488,56 @@
         <v>0</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -1813,23 +1557,11 @@
       <c r="A8" s="3"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C3DFCCB6-F847-9744-B65E-7CF60232C620}">
-          <x14:formula1>
-            <xm:f>menus!$C$2:$C$16</xm:f>
-          </x14:formula1>
-          <xm:sqref>C2:C3</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -1842,10 +1574,10 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="15.83203125" customWidth="1"/>
-    <col min="4" max="4" width="25.83203125" customWidth="1"/>
-    <col min="5" max="5" width="30.83203125" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" customWidth="1"/>
+    <col min="5" max="5" width="20.83203125" customWidth="1"/>
     <col min="6" max="6" width="22.83203125" customWidth="1"/>
-    <col min="7" max="7" width="20.83203125" customWidth="1"/>
+    <col min="7" max="7" width="23.83203125" customWidth="1"/>
     <col min="8" max="10" width="25.83203125" customWidth="1"/>
     <col min="11" max="11" width="22.83203125" customWidth="1"/>
     <col min="12" max="12" width="20.83203125" customWidth="1"/>
@@ -1857,7 +1589,7 @@
         <v>4</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>104</v>
+        <v>53</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>3</v>
@@ -1866,22 +1598,22 @@
         <v>5</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>106</v>
+        <v>55</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="H1" s="7" t="s">
         <v>6</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>95</v>
+        <v>50</v>
       </c>
       <c r="J1" s="7" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="K1" s="7" t="s">
         <v>7</v>
@@ -1893,120 +1625,96 @@
         <v>8</v>
       </c>
       <c r="N1" s="7" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="O1" s="7" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>24</v>
+        <v>63</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>88</v>
-      </c>
       <c r="K2" s="1" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>24</v>
+        <v>63</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>103</v>
+        <v>52</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>89</v>
+        <v>44</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>87</v>
+        <v>42</v>
       </c>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
       <c r="N3" s="1" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{88DE7120-2FCE-364C-A552-C3E89AB1A2C4}">
-          <x14:formula1>
-            <xm:f>menus!$C$2:$C$16</xm:f>
-          </x14:formula1>
-          <xm:sqref>C2:C3</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{FAA51CD0-43E0-A943-8055-0C5FB8D6C680}">
-          <x14:formula1>
-            <xm:f>menus!$G$2:$G$18</xm:f>
-          </x14:formula1>
-          <xm:sqref>D2:D3</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{E5F9E90A-E21A-8A41-BB6A-B83D71712C77}">
-          <x14:formula1>
-            <xm:f>menus!$E$2:$E$8</xm:f>
-          </x14:formula1>
-          <xm:sqref>E2:F3</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2033,77 +1741,77 @@
         <v>4</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>90</v>
+        <v>45</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>91</v>
+        <v>46</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>92</v>
+        <v>47</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>93</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>102</v>
+        <v>51</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>88</v>
+        <v>43</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>94</v>
+        <v>49</v>
       </c>
       <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>103</v>
+        <v>52</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>89</v>
+        <v>44</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>94</v>
+        <v>49</v>
       </c>
       <c r="E5" s="1"/>
     </row>
@@ -2119,9 +1827,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD8FB4E8-B9B5-D24A-91D9-6FACBB875664}">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2130,46 +1836,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="G1" s="13" t="s">
+      <c r="D1" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="I1" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="J1" s="13" t="s">
-        <v>31</v>
+      <c r="H1" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>21</v>
+        <v>64</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1">
@@ -2179,21 +1885,21 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>87</v>
+        <v>42</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>21</v>
+        <v>64</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1">
@@ -2203,10 +1909,10 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -2236,249 +1942,46 @@
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{14833FDB-C112-704E-9CEE-46E5E14AD65D}">
-          <x14:formula1>
-            <xm:f>menus!$C$2:$C$16</xm:f>
-          </x14:formula1>
-          <xm:sqref>B2:B3</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8B6688A4-70D6-FC45-94AF-02BA5F718A94}">
-          <x14:formula1>
-            <xm:f>menus!$I$2:$I$5</xm:f>
-          </x14:formula1>
-          <xm:sqref>C2:C3</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A27DA9FB-C6DE-DD43-83A1-C14B1BF5FE4D}">
-  <dimension ref="A1:I18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7359C2B5-7D36-5048-B20A-75ECED0C559D}">
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.83203125" customWidth="1"/>
-    <col min="2" max="2" width="1.83203125" customWidth="1"/>
-    <col min="3" max="3" width="15.83203125" customWidth="1"/>
-    <col min="4" max="4" width="1.83203125" customWidth="1"/>
-    <col min="5" max="5" width="63.83203125" customWidth="1"/>
-    <col min="6" max="6" width="1.83203125" customWidth="1"/>
-    <col min="7" max="7" width="44.83203125" customWidth="1"/>
-    <col min="8" max="8" width="1.83203125" customWidth="1"/>
-    <col min="9" max="9" width="15.83203125" customWidth="1"/>
+    <col min="2" max="2" width="30.83203125" customWidth="1"/>
+    <col min="3" max="3" width="40.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="I2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>98</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="G3" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="I3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>99</v>
-      </c>
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="9" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="G4" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="I4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>100</v>
-      </c>
-      <c r="C5" t="s">
-        <v>54</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G5" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="I5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>101</v>
-      </c>
-      <c r="C6" t="s">
-        <v>55</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="G6" s="10" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C7" t="s">
-        <v>56</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="G7" s="10" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C8" t="s">
-        <v>57</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="G8" s="10" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C9" t="s">
-        <v>58</v>
-      </c>
-      <c r="G9" s="10" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C10" t="s">
-        <v>59</v>
-      </c>
-      <c r="G10" s="10" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C11" t="s">
-        <v>60</v>
-      </c>
-      <c r="G11" s="10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C12" t="s">
-        <v>61</v>
-      </c>
-      <c r="G12" s="10" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C13" t="s">
-        <v>62</v>
-      </c>
-      <c r="G13" s="10" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C14" t="s">
-        <v>63</v>
-      </c>
-      <c r="G14" s="10" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C15" t="s">
-        <v>64</v>
-      </c>
-      <c r="G15" s="10" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C16" t="s">
-        <v>65</v>
-      </c>
-      <c r="G16" s="10" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="17" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G17" s="10" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="18" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G18" s="10" t="s">
-        <v>84</v>
-      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="1"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="5">
+  <tableParts count="1">
     <tablePart r:id="rId1"/>
-    <tablePart r:id="rId2"/>
-    <tablePart r:id="rId3"/>
-    <tablePart r:id="rId4"/>
-    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated mac version to 0.0.0.0.16
</commit_message>
<xml_diff>
--- a/examples/vpc.xlsx
+++ b/examples/vpc.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jww/Developer/python/terraformer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F149B92-FADB-414C-98C3-67AA253559F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A27A3F1-4C5C-3549-910F-8ADA3D1EFDDB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2840" yWindow="460" windowWidth="25600" windowHeight="14700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14700" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="vpcheaders" sheetId="6" r:id="rId1"/>
     <sheet name="vpcaddresses" sheetId="51" r:id="rId2"/>
-    <sheet name="subnets" sheetId="26" r:id="rId3"/>
-    <sheet name="instances" sheetId="27" r:id="rId4"/>
-    <sheet name="networkinterfaces" sheetId="50" r:id="rId5"/>
-    <sheet name="volumes" sheetId="49" r:id="rId6"/>
-    <sheet name="images" sheetId="52" r:id="rId7"/>
+    <sheet name="vpcroutes" sheetId="53" r:id="rId3"/>
+    <sheet name="subnets" sheetId="26" r:id="rId4"/>
+    <sheet name="instances" sheetId="27" r:id="rId5"/>
+    <sheet name="networkinterfaces" sheetId="50" r:id="rId6"/>
+    <sheet name="volumes" sheetId="49" r:id="rId7"/>
+    <sheet name="images" sheetId="52" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="69">
   <si>
     <t>public_gateway</t>
   </si>
@@ -238,6 +239,12 @@
   </si>
   <si>
     <t>*operating_system</t>
+  </si>
+  <si>
+    <t>*destination</t>
+  </si>
+  <si>
+    <t>*next_hop</t>
   </si>
 </sst>
 </file>
@@ -393,7 +400,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="66">
+  <dxfs count="73">
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -614,6 +621,33 @@
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4"/>
         </patternFill>
       </fill>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -952,13 +986,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{7215B7F5-B70C-6B42-84D7-6729B99B446D}" name="Table8" displayName="Table8" ref="A1:F3" totalsRowShown="0" headerRowDxfId="65" dataDxfId="64" tableBorderDxfId="63">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{7215B7F5-B70C-6B42-84D7-6729B99B446D}" name="Table8" displayName="Table8" ref="A1:F3" totalsRowShown="0" headerRowDxfId="72" dataDxfId="71" tableBorderDxfId="70">
   <autoFilter ref="A1:F3" xr:uid="{529F7172-ECCA-724F-9B2D-5A6C4B69CB3C}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{887BA8C8-9946-8A42-98DF-3633CAED0C28}" name="*name" dataDxfId="62"/>
-    <tableColumn id="5" xr3:uid="{5CEDAE6E-6D63-FE4C-B1E4-8EBD674619A5}" name="default_network_acl" dataDxfId="61"/>
+    <tableColumn id="1" xr3:uid="{887BA8C8-9946-8A42-98DF-3633CAED0C28}" name="*name" dataDxfId="69"/>
+    <tableColumn id="5" xr3:uid="{5CEDAE6E-6D63-FE4C-B1E4-8EBD674619A5}" name="default_network_acl" dataDxfId="68"/>
     <tableColumn id="3" xr3:uid="{D2048242-D53A-2A48-924A-8019052FD266}" name="address_prefix_management"/>
-    <tableColumn id="2" xr3:uid="{A41B6291-1C2E-AB41-A22B-93622DC498B2}" name="classic_access" dataDxfId="60"/>
+    <tableColumn id="2" xr3:uid="{A41B6291-1C2E-AB41-A22B-93622DC498B2}" name="classic_access" dataDxfId="67"/>
     <tableColumn id="4" xr3:uid="{9675255E-64F1-104E-BCF2-8AF88D430E4B}" name="resource_group"/>
     <tableColumn id="7" xr3:uid="{DF1FC027-D537-CB40-BAA8-AEAEE8D9E2C7}" name="tags"/>
   </tableColumns>
@@ -967,19 +1001,33 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{80420FF8-12AA-D148-A5E9-F305380E9AC4}" name="Table82" displayName="Table82" ref="A1:D3" totalsRowShown="0" headerRowDxfId="59" dataDxfId="58" tableBorderDxfId="57">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{80420FF8-12AA-D148-A5E9-F305380E9AC4}" name="Table82" displayName="Table82" ref="A1:D3" totalsRowShown="0" headerRowDxfId="66" dataDxfId="65" tableBorderDxfId="64">
   <autoFilter ref="A1:D3" xr:uid="{9C9BAFE8-9631-CE45-93B1-83DB9C4014D5}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{C6C9ADE6-AC77-4944-9C6C-9D136392888D}" name="*name" dataDxfId="56"/>
-    <tableColumn id="5" xr3:uid="{0731D78F-C6D2-8948-BD0A-FB61D3B47F6C}" name="*vpc" dataDxfId="55"/>
+    <tableColumn id="1" xr3:uid="{C6C9ADE6-AC77-4944-9C6C-9D136392888D}" name="*name" dataDxfId="63"/>
+    <tableColumn id="5" xr3:uid="{0731D78F-C6D2-8948-BD0A-FB61D3B47F6C}" name="*vpc" dataDxfId="62"/>
     <tableColumn id="3" xr3:uid="{A408C4C2-23CE-B443-BA1D-7440072D5651}" name="*zone"/>
-    <tableColumn id="2" xr3:uid="{F0825E63-100E-584C-B142-E4481E9F997C}" name="*cidr" dataDxfId="54"/>
+    <tableColumn id="2" xr3:uid="{F0825E63-100E-584C-B142-E4481E9F997C}" name="*cidr" dataDxfId="61"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{E7E4E482-6BB9-E248-AF8D-C5304BC1A44F}" name="Table3236" displayName="Table3236" ref="A1:E3" totalsRowShown="0" headerRowDxfId="60" dataDxfId="59">
+  <autoFilter ref="A1:E3" xr:uid="{DC08D300-10E5-4A45-A724-480E99186CDC}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{60C065E1-55B2-104C-9BD3-648FFAC30A51}" name="*name" dataDxfId="58"/>
+    <tableColumn id="3" xr3:uid="{8BD05EA0-AFD7-AF41-B934-9ECEE2438312}" name="*vpc" dataDxfId="57"/>
+    <tableColumn id="2" xr3:uid="{92355D65-8FB2-FA47-80DC-D34EF9FEADBD}" name="*zone" dataDxfId="56"/>
+    <tableColumn id="4" xr3:uid="{EF21D846-0B2C-9441-B0FD-2EA28736C729}" name="*destination" dataDxfId="55"/>
+    <tableColumn id="5" xr3:uid="{7D2B7989-C527-9D46-A034-89A1FB4BA0D5}" name="*next_hop" dataDxfId="54"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{76790F31-1453-B641-9754-80A9D247EA0F}" name="Table6" displayName="Table6" ref="A1:K3" totalsRowShown="0" headerRowDxfId="53" dataDxfId="52">
   <autoFilter ref="A1:K3" xr:uid="{9725F296-5A96-A949-A782-B4A2B65596C4}"/>
   <tableColumns count="11">
@@ -999,7 +1047,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{3F1E4605-7351-6A4A-9807-A10DCEAD79B7}" name="Table7" displayName="Table7" ref="A1:O3" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39">
   <autoFilter ref="A1:O3" xr:uid="{4F0FA061-E3B2-AB4E-A276-92C803DED60C}"/>
   <tableColumns count="15">
@@ -1023,7 +1071,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{81661C9C-F36C-2E41-BF2C-12573A860276}" name="Table75" displayName="Table75" ref="A1:E5" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
   <autoFilter ref="A1:E5" xr:uid="{4F0FA061-E3B2-AB4E-A276-92C803DED60C}"/>
   <tableColumns count="5">
@@ -1037,7 +1085,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C451A855-5250-674B-8039-E23EC3348E96}" name="Table11" displayName="Table11" ref="A1:J3" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
   <autoFilter ref="A1:J3" xr:uid="{8CD156A6-A66F-1245-BCD2-9FAE26A0A77C}"/>
   <tableColumns count="10">
@@ -1056,7 +1104,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5CC6AE3F-9734-ED45-8903-103E4A3651C5}" name="Table323" displayName="Table323" ref="A1:C3" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
   <autoFilter ref="A1:C3" xr:uid="{DC08D300-10E5-4A45-A724-480E99186CDC}"/>
   <tableColumns count="3">
@@ -1333,7 +1381,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D5606E7-1677-4EE2-808E-F237A1A9F8B6}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1451,6 +1499,58 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E341B84-0FAA-F64A-AA01-BA6699EAC299}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="3" width="15.83203125" customWidth="1"/>
+    <col min="4" max="5" width="20.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58E633D9-8336-4776-A01F-1859C551A2C4}">
   <dimension ref="A1:K8"/>
   <sheetViews>
@@ -1565,7 +1665,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69A31708-3A2C-4ADA-B3E5-8A1B18923F2A}">
   <dimension ref="A1:O3"/>
   <sheetViews>
@@ -1718,7 +1818,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FCD209A-28DD-7845-952F-4118CB029C17}">
   <dimension ref="A1:E5"/>
   <sheetViews>
@@ -1823,7 +1923,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD8FB4E8-B9B5-D24A-91D9-6FACBB875664}">
   <dimension ref="A1:J4"/>
   <sheetViews>
@@ -1945,7 +2045,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7359C2B5-7D36-5048-B20A-75ECED0C559D}">
   <dimension ref="A1:C3"/>
   <sheetViews>

</xml_diff>

<commit_message>
updated mac version to 0.0.0.0.18
</commit_message>
<xml_diff>
--- a/examples/vpc.xlsx
+++ b/examples/vpc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jww/Developer/python/terraformer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C1A1958-3A3C-A042-BDDD-984FC50E897A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{850EC2E4-B4DE-A84D-9A26-3CE3946DA39C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="480" windowWidth="25600" windowHeight="14700" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="vpcheaders" sheetId="6" r:id="rId1"/>
@@ -18,8 +18,8 @@
     <sheet name="vpcroutes" sheetId="53" r:id="rId3"/>
     <sheet name="subnets" sheetId="26" r:id="rId4"/>
     <sheet name="instances" sheetId="27" r:id="rId5"/>
-    <sheet name="networkinterfaces" sheetId="50" r:id="rId6"/>
-    <sheet name="volumes" sheetId="49" r:id="rId7"/>
+    <sheet name="volumes" sheetId="49" r:id="rId6"/>
+    <sheet name="networkinterfaces" sheetId="50" r:id="rId7"/>
     <sheet name="images" sheetId="52" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="74">
   <si>
     <t>public_gateway</t>
   </si>
@@ -142,12 +142,6 @@
     <t>fip1</t>
   </si>
   <si>
-    <t>boot_volume_name</t>
-  </si>
-  <si>
-    <t>boot_volume_encryption</t>
-  </si>
-  <si>
     <t>acl1</t>
   </si>
   <si>
@@ -163,12 +157,6 @@
     <t>resource_controller_url</t>
   </si>
   <si>
-    <t>volume1</t>
-  </si>
-  <si>
-    <t>volume2</t>
-  </si>
-  <si>
     <t>vsi1nic1</t>
   </si>
   <si>
@@ -193,12 +181,6 @@
     <t>*primary_network_interface</t>
   </si>
   <si>
-    <t>vsi1nic0primary</t>
-  </si>
-  <si>
-    <t>vsi2nic0primary</t>
-  </si>
-  <si>
     <t>*vpc</t>
   </si>
   <si>
@@ -245,6 +227,39 @@
   </si>
   <si>
     <t>*next_hop</t>
+  </si>
+  <si>
+    <t>*attachment_type</t>
+  </si>
+  <si>
+    <t>data</t>
+  </si>
+  <si>
+    <t>boot</t>
+  </si>
+  <si>
+    <t>vsi1boot</t>
+  </si>
+  <si>
+    <t>vsi2boot</t>
+  </si>
+  <si>
+    <t>vsi1data</t>
+  </si>
+  <si>
+    <t>vsi2data</t>
+  </si>
+  <si>
+    <t>boot_volume</t>
+  </si>
+  <si>
+    <t>vsi1primarynic</t>
+  </si>
+  <si>
+    <t>vsi2primarynic</t>
+  </si>
+  <si>
+    <t>general-purpose</t>
   </si>
 </sst>
 </file>
@@ -400,49 +415,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="73">
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
+  <dxfs count="74">
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -508,6 +481,51 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -986,13 +1004,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{7215B7F5-B70C-6B42-84D7-6729B99B446D}" name="Table8" displayName="Table8" ref="A1:F3" totalsRowShown="0" headerRowDxfId="72" dataDxfId="71" tableBorderDxfId="70">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{7215B7F5-B70C-6B42-84D7-6729B99B446D}" name="Table8" displayName="Table8" ref="A1:F3" totalsRowShown="0" headerRowDxfId="73" dataDxfId="72" tableBorderDxfId="71">
   <autoFilter ref="A1:F3" xr:uid="{529F7172-ECCA-724F-9B2D-5A6C4B69CB3C}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{887BA8C8-9946-8A42-98DF-3633CAED0C28}" name="*name" dataDxfId="69"/>
-    <tableColumn id="5" xr3:uid="{5CEDAE6E-6D63-FE4C-B1E4-8EBD674619A5}" name="default_network_acl" dataDxfId="68"/>
+    <tableColumn id="1" xr3:uid="{887BA8C8-9946-8A42-98DF-3633CAED0C28}" name="*name" dataDxfId="70"/>
+    <tableColumn id="5" xr3:uid="{5CEDAE6E-6D63-FE4C-B1E4-8EBD674619A5}" name="default_network_acl" dataDxfId="69"/>
     <tableColumn id="3" xr3:uid="{D2048242-D53A-2A48-924A-8019052FD266}" name="address_prefix_management"/>
-    <tableColumn id="2" xr3:uid="{A41B6291-1C2E-AB41-A22B-93622DC498B2}" name="classic_access" dataDxfId="67"/>
+    <tableColumn id="2" xr3:uid="{A41B6291-1C2E-AB41-A22B-93622DC498B2}" name="classic_access" dataDxfId="68"/>
     <tableColumn id="4" xr3:uid="{9675255E-64F1-104E-BCF2-8AF88D430E4B}" name="resource_group"/>
     <tableColumn id="7" xr3:uid="{DF1FC027-D537-CB40-BAA8-AEAEE8D9E2C7}" name="tags"/>
   </tableColumns>
@@ -1001,104 +1019,105 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{80420FF8-12AA-D148-A5E9-F305380E9AC4}" name="Table82" displayName="Table82" ref="A1:D3" totalsRowShown="0" headerRowDxfId="66" dataDxfId="65" tableBorderDxfId="64">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{80420FF8-12AA-D148-A5E9-F305380E9AC4}" name="Table82" displayName="Table82" ref="A1:D3" totalsRowShown="0" headerRowDxfId="67" dataDxfId="66" tableBorderDxfId="65">
   <autoFilter ref="A1:D3" xr:uid="{9C9BAFE8-9631-CE45-93B1-83DB9C4014D5}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{C6C9ADE6-AC77-4944-9C6C-9D136392888D}" name="*name" dataDxfId="63"/>
-    <tableColumn id="5" xr3:uid="{0731D78F-C6D2-8948-BD0A-FB61D3B47F6C}" name="*vpc" dataDxfId="62"/>
+    <tableColumn id="1" xr3:uid="{C6C9ADE6-AC77-4944-9C6C-9D136392888D}" name="*name" dataDxfId="64"/>
+    <tableColumn id="5" xr3:uid="{0731D78F-C6D2-8948-BD0A-FB61D3B47F6C}" name="*vpc" dataDxfId="63"/>
     <tableColumn id="3" xr3:uid="{A408C4C2-23CE-B443-BA1D-7440072D5651}" name="*zone"/>
-    <tableColumn id="2" xr3:uid="{F0825E63-100E-584C-B142-E4481E9F997C}" name="*cidr" dataDxfId="61"/>
+    <tableColumn id="2" xr3:uid="{F0825E63-100E-584C-B142-E4481E9F997C}" name="*cidr" dataDxfId="62"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{E7E4E482-6BB9-E248-AF8D-C5304BC1A44F}" name="Table3236" displayName="Table3236" ref="A1:E3" totalsRowShown="0" headerRowDxfId="60" dataDxfId="59">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{E7E4E482-6BB9-E248-AF8D-C5304BC1A44F}" name="Table3236" displayName="Table3236" ref="A1:E3" totalsRowShown="0" headerRowDxfId="61" dataDxfId="60">
   <autoFilter ref="A1:E3" xr:uid="{DC08D300-10E5-4A45-A724-480E99186CDC}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{60C065E1-55B2-104C-9BD3-648FFAC30A51}" name="*name" dataDxfId="58"/>
-    <tableColumn id="3" xr3:uid="{8BD05EA0-AFD7-AF41-B934-9ECEE2438312}" name="*vpc" dataDxfId="57"/>
-    <tableColumn id="2" xr3:uid="{92355D65-8FB2-FA47-80DC-D34EF9FEADBD}" name="*zone" dataDxfId="56"/>
-    <tableColumn id="4" xr3:uid="{EF21D846-0B2C-9441-B0FD-2EA28736C729}" name="*destination" dataDxfId="55"/>
-    <tableColumn id="5" xr3:uid="{7D2B7989-C527-9D46-A034-89A1FB4BA0D5}" name="*next_hop" dataDxfId="54"/>
+    <tableColumn id="1" xr3:uid="{60C065E1-55B2-104C-9BD3-648FFAC30A51}" name="*name" dataDxfId="59"/>
+    <tableColumn id="3" xr3:uid="{8BD05EA0-AFD7-AF41-B934-9ECEE2438312}" name="*vpc" dataDxfId="58"/>
+    <tableColumn id="2" xr3:uid="{92355D65-8FB2-FA47-80DC-D34EF9FEADBD}" name="*zone" dataDxfId="57"/>
+    <tableColumn id="4" xr3:uid="{EF21D846-0B2C-9441-B0FD-2EA28736C729}" name="*destination" dataDxfId="56"/>
+    <tableColumn id="5" xr3:uid="{7D2B7989-C527-9D46-A034-89A1FB4BA0D5}" name="*next_hop" dataDxfId="55"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{76790F31-1453-B641-9754-80A9D247EA0F}" name="Table6" displayName="Table6" ref="A1:K3" totalsRowShown="0" headerRowDxfId="53" dataDxfId="52">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{76790F31-1453-B641-9754-80A9D247EA0F}" name="Table6" displayName="Table6" ref="A1:K3" totalsRowShown="0" headerRowDxfId="54" dataDxfId="53">
   <autoFilter ref="A1:K3" xr:uid="{9725F296-5A96-A949-A782-B4A2B65596C4}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{1E9E58AF-C46F-2140-86A4-81396AD00F15}" name="*name" dataDxfId="51"/>
-    <tableColumn id="11" xr3:uid="{9C2673D8-AB9A-9645-A3ED-D9B779022434}" name="*vpc" dataDxfId="50"/>
-    <tableColumn id="2" xr3:uid="{D989FA97-121E-ED4E-9CA5-25D303F38C24}" name="*zone" dataDxfId="49"/>
-    <tableColumn id="3" xr3:uid="{9DE77DE5-F660-7D4C-BC60-2B014D5E01EB}" name="ipv4_cidr_block" dataDxfId="48"/>
-    <tableColumn id="4" xr3:uid="{42D706D7-A721-6D49-8189-9A181B88E99F}" name="total_ipv4_address_count" dataDxfId="47"/>
-    <tableColumn id="5" xr3:uid="{215941D8-E315-5044-8E51-E2FEE9B95908}" name="ip_version" dataDxfId="46"/>
-    <tableColumn id="6" xr3:uid="{7CE7912A-5366-5A4D-9CAD-006BE9E02B39}" name="network_acl" dataDxfId="45"/>
-    <tableColumn id="7" xr3:uid="{87A1EA58-5C4B-0443-A650-07ABED9C6F31}" name="public_gateway" dataDxfId="44"/>
-    <tableColumn id="8" xr3:uid="{718DFD83-0842-7749-8498-7034DCF9F245}" name="create_timeout" dataDxfId="43"/>
-    <tableColumn id="9" xr3:uid="{6E310B89-982B-B743-8106-2EEBD001DB52}" name="update_timeout" dataDxfId="42"/>
-    <tableColumn id="10" xr3:uid="{16A0C085-1B24-8740-BCEF-FC5FBADEF6C0}" name="delete_timeout" dataDxfId="41"/>
+    <tableColumn id="1" xr3:uid="{1E9E58AF-C46F-2140-86A4-81396AD00F15}" name="*name" dataDxfId="52"/>
+    <tableColumn id="11" xr3:uid="{9C2673D8-AB9A-9645-A3ED-D9B779022434}" name="*vpc" dataDxfId="51"/>
+    <tableColumn id="2" xr3:uid="{D989FA97-121E-ED4E-9CA5-25D303F38C24}" name="*zone" dataDxfId="50"/>
+    <tableColumn id="3" xr3:uid="{9DE77DE5-F660-7D4C-BC60-2B014D5E01EB}" name="ipv4_cidr_block" dataDxfId="49"/>
+    <tableColumn id="4" xr3:uid="{42D706D7-A721-6D49-8189-9A181B88E99F}" name="total_ipv4_address_count" dataDxfId="48"/>
+    <tableColumn id="5" xr3:uid="{215941D8-E315-5044-8E51-E2FEE9B95908}" name="ip_version" dataDxfId="47"/>
+    <tableColumn id="6" xr3:uid="{7CE7912A-5366-5A4D-9CAD-006BE9E02B39}" name="network_acl" dataDxfId="46"/>
+    <tableColumn id="7" xr3:uid="{87A1EA58-5C4B-0443-A650-07ABED9C6F31}" name="public_gateway" dataDxfId="45"/>
+    <tableColumn id="8" xr3:uid="{718DFD83-0842-7749-8498-7034DCF9F245}" name="create_timeout" dataDxfId="44"/>
+    <tableColumn id="9" xr3:uid="{6E310B89-982B-B743-8106-2EEBD001DB52}" name="update_timeout" dataDxfId="43"/>
+    <tableColumn id="10" xr3:uid="{16A0C085-1B24-8740-BCEF-FC5FBADEF6C0}" name="delete_timeout" dataDxfId="42"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{3F1E4605-7351-6A4A-9807-A10DCEAD79B7}" name="Table7" displayName="Table7" ref="A1:O3" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39">
-  <autoFilter ref="A1:O3" xr:uid="{4F0FA061-E3B2-AB4E-A276-92C803DED60C}"/>
-  <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{B447E9AB-445F-0242-8396-EEAA92074797}" name="*name" dataDxfId="38"/>
-    <tableColumn id="7" xr3:uid="{AECA3B2B-972B-2947-B76F-3FE48277F64A}" name="*vpc" dataDxfId="37"/>
-    <tableColumn id="2" xr3:uid="{E6843232-FC96-094F-809F-D9A2D9A3F5CB}" name="*zone" dataDxfId="36"/>
-    <tableColumn id="3" xr3:uid="{E7DB5053-DB66-CF46-AB33-5A411FF07264}" name="*profile" dataDxfId="35"/>
-    <tableColumn id="4" xr3:uid="{F65626CD-0D0E-D748-9934-00DB105BEEAC}" name="*image" dataDxfId="34"/>
-    <tableColumn id="14" xr3:uid="{1A5FD37C-8F61-7B49-9DE5-C024F0CC91E5}" name="boot_volume_name" dataDxfId="33"/>
-    <tableColumn id="5" xr3:uid="{436C5517-AF19-1946-8EE7-03879E1F2944}" name="boot_volume_encryption" dataDxfId="32"/>
-    <tableColumn id="6" xr3:uid="{FFE24952-72F9-9D47-8A4B-2813BCCB260E}" name="*keys" dataDxfId="31"/>
-    <tableColumn id="9" xr3:uid="{A03604D8-6E33-4249-A9DE-BF8870E3D90B}" name="*primary_network_interface" dataDxfId="30"/>
-    <tableColumn id="10" xr3:uid="{438F95E2-E2D5-1E49-9852-4B915078693E}" name="network_interfaces" dataDxfId="29"/>
-    <tableColumn id="19" xr3:uid="{6293540A-4A05-0E4A-99ED-C75D3F46ECCF}" name="volumes" dataDxfId="28"/>
-    <tableColumn id="18" xr3:uid="{8C2D6431-BD15-6849-BBE1-C0EF1B26E51A}" name="user_data" dataDxfId="27"/>
-    <tableColumn id="17" xr3:uid="{8C7E9F80-830B-174D-9411-54916978023E}" name="resource_group" dataDxfId="26"/>
-    <tableColumn id="12" xr3:uid="{E2511928-0801-3546-B6BA-F9C8EF98BBC6}" name="create_timeout" dataDxfId="25"/>
-    <tableColumn id="13" xr3:uid="{F33A3F16-B62A-EC4B-BC5D-BAA56655B743}" name="delete_timeout" dataDxfId="24"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{3F1E4605-7351-6A4A-9807-A10DCEAD79B7}" name="Table7" displayName="Table7" ref="A1:N3" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
+  <autoFilter ref="A1:N3" xr:uid="{4F0FA061-E3B2-AB4E-A276-92C803DED60C}"/>
+  <tableColumns count="14">
+    <tableColumn id="1" xr3:uid="{B447E9AB-445F-0242-8396-EEAA92074797}" name="*name" dataDxfId="39"/>
+    <tableColumn id="7" xr3:uid="{AECA3B2B-972B-2947-B76F-3FE48277F64A}" name="*vpc" dataDxfId="38"/>
+    <tableColumn id="2" xr3:uid="{E6843232-FC96-094F-809F-D9A2D9A3F5CB}" name="*zone" dataDxfId="37"/>
+    <tableColumn id="3" xr3:uid="{E7DB5053-DB66-CF46-AB33-5A411FF07264}" name="*profile" dataDxfId="36"/>
+    <tableColumn id="4" xr3:uid="{F65626CD-0D0E-D748-9934-00DB105BEEAC}" name="*image" dataDxfId="35"/>
+    <tableColumn id="14" xr3:uid="{1A5FD37C-8F61-7B49-9DE5-C024F0CC91E5}" name="boot_volume" dataDxfId="34"/>
+    <tableColumn id="6" xr3:uid="{FFE24952-72F9-9D47-8A4B-2813BCCB260E}" name="*keys" dataDxfId="33"/>
+    <tableColumn id="9" xr3:uid="{A03604D8-6E33-4249-A9DE-BF8870E3D90B}" name="*primary_network_interface" dataDxfId="32"/>
+    <tableColumn id="10" xr3:uid="{438F95E2-E2D5-1E49-9852-4B915078693E}" name="network_interfaces" dataDxfId="31"/>
+    <tableColumn id="19" xr3:uid="{6293540A-4A05-0E4A-99ED-C75D3F46ECCF}" name="volumes" dataDxfId="30"/>
+    <tableColumn id="18" xr3:uid="{8C2D6431-BD15-6849-BBE1-C0EF1B26E51A}" name="user_data" dataDxfId="29"/>
+    <tableColumn id="17" xr3:uid="{8C7E9F80-830B-174D-9411-54916978023E}" name="resource_group" dataDxfId="28"/>
+    <tableColumn id="12" xr3:uid="{E2511928-0801-3546-B6BA-F9C8EF98BBC6}" name="create_timeout" dataDxfId="27"/>
+    <tableColumn id="13" xr3:uid="{F33A3F16-B62A-EC4B-BC5D-BAA56655B743}" name="delete_timeout" dataDxfId="26"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{81661C9C-F36C-2E41-BF2C-12573A860276}" name="Table75" displayName="Table75" ref="A1:E5" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
-  <autoFilter ref="A1:E5" xr:uid="{4F0FA061-E3B2-AB4E-A276-92C803DED60C}"/>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{95E267F3-7620-8C4D-AFC7-4EB9DFAE946B}" name="*name" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{C13CAAAB-1F09-F442-B06D-36989DBA835A}" name="*instance" dataDxfId="20"/>
-    <tableColumn id="8" xr3:uid="{B55BB537-FA6A-D04D-99CC-63555EFADEB6}" name="*subnet" dataDxfId="19"/>
-    <tableColumn id="11" xr3:uid="{346BFF31-BC5B-C647-89BB-72AE7861274F}" name="security_groups" dataDxfId="18"/>
-    <tableColumn id="7" xr3:uid="{80D936B9-9EFA-6C4B-BF5E-9435B5B9B191}" name="floating_ip" dataDxfId="17"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C451A855-5250-674B-8039-E23EC3348E96}" name="Table11" displayName="Table11" ref="A1:L6" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
+  <autoFilter ref="A1:L6" xr:uid="{8CD156A6-A66F-1245-BCD2-9FAE26A0A77C}"/>
+  <tableColumns count="12">
+    <tableColumn id="1" xr3:uid="{CDC18A34-D228-8E41-90CD-62AD9ACAF229}" name="*name" dataDxfId="23"/>
+    <tableColumn id="11" xr3:uid="{314C1371-3329-EA42-AB4C-3D8F83971269}" name="*instance" dataDxfId="22"/>
+    <tableColumn id="12" xr3:uid="{1BF2A89E-63CD-FA4D-B1ED-9A3CD987DFF3}" name="*attachment_type" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{480E110A-7DA0-1A46-B19A-DAB8291BA972}" name="*zone" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{1B453B9B-A3A5-5948-96F3-62C87F788C3A}" name="*profile" dataDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{6CC60290-7B72-D343-A43F-F0F762500CF4}" name="iops" dataDxfId="18"/>
+    <tableColumn id="5" xr3:uid="{45C880C0-FF4F-2F4A-919A-124DB93E5010}" name="capacity" dataDxfId="17"/>
+    <tableColumn id="6" xr3:uid="{787D8375-0B24-5F42-A273-3093BD8B60EC}" name="encryption_key" dataDxfId="16"/>
+    <tableColumn id="7" xr3:uid="{392944E6-6831-6F41-86DE-438B3577B0C6}" name="resource_group" dataDxfId="15"/>
+    <tableColumn id="8" xr3:uid="{2D73C361-1CE6-FF4D-BC45-651F77AC5BE1}" name="resource_controller_url" dataDxfId="14"/>
+    <tableColumn id="9" xr3:uid="{DC38DEC2-7381-DD45-A09D-F3050D08CA1E}" name="create_timeout" dataDxfId="13"/>
+    <tableColumn id="10" xr3:uid="{63225B45-4949-7A45-9F18-531EB8888D63}" name="delete_timeout" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C451A855-5250-674B-8039-E23EC3348E96}" name="Table11" displayName="Table11" ref="A1:J3" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
-  <autoFilter ref="A1:J3" xr:uid="{8CD156A6-A66F-1245-BCD2-9FAE26A0A77C}"/>
-  <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{CDC18A34-D228-8E41-90CD-62AD9ACAF229}" name="*name" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{480E110A-7DA0-1A46-B19A-DAB8291BA972}" name="*zone" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{1B453B9B-A3A5-5948-96F3-62C87F788C3A}" name="*profile" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{6CC60290-7B72-D343-A43F-F0F762500CF4}" name="iops" dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{45C880C0-FF4F-2F4A-919A-124DB93E5010}" name="capacity" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{787D8375-0B24-5F42-A273-3093BD8B60EC}" name="encryption_key" dataDxfId="9"/>
-    <tableColumn id="7" xr3:uid="{392944E6-6831-6F41-86DE-438B3577B0C6}" name="resource_group" dataDxfId="8"/>
-    <tableColumn id="8" xr3:uid="{2D73C361-1CE6-FF4D-BC45-651F77AC5BE1}" name="resource_controller_url" dataDxfId="7"/>
-    <tableColumn id="9" xr3:uid="{DC38DEC2-7381-DD45-A09D-F3050D08CA1E}" name="create_timeout" dataDxfId="6"/>
-    <tableColumn id="10" xr3:uid="{63225B45-4949-7A45-9F18-531EB8888D63}" name="delete_timeout" dataDxfId="5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{81661C9C-F36C-2E41-BF2C-12573A860276}" name="Table75" displayName="Table75" ref="A1:E6" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:E6" xr:uid="{4F0FA061-E3B2-AB4E-A276-92C803DED60C}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{95E267F3-7620-8C4D-AFC7-4EB9DFAE946B}" name="*name" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{C13CAAAB-1F09-F442-B06D-36989DBA835A}" name="*instance" dataDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{B55BB537-FA6A-D04D-99CC-63555EFADEB6}" name="*subnet" dataDxfId="7"/>
+    <tableColumn id="11" xr3:uid="{346BFF31-BC5B-C647-89BB-72AE7861274F}" name="security_groups" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{80D936B9-9EFA-6C4B-BF5E-9435B5B9B191}" name="floating_ip" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1381,7 +1400,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D5606E7-1677-4EE2-808E-F237A1A9F8B6}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1399,7 +1418,7 @@
         <v>16</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D1" s="8" t="s">
         <v>17</v>
@@ -1416,10 +1435,10 @@
         <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C2" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -1452,18 +1471,18 @@
         <v>4</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>3</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B2" t="s">
         <v>26</v>
@@ -1472,12 +1491,12 @@
         <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>26</v>
@@ -1486,7 +1505,7 @@
         <v>13</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1515,16 +1534,16 @@
         <v>4</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C1" s="11" t="s">
         <v>3</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -1568,7 +1587,7 @@
         <v>4</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C1" t="s">
         <v>3</v>
@@ -1668,9 +1687,9 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69A31708-3A2C-4ADA-B3E5-8A1B18923F2A}">
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1685,12 +1704,12 @@
     <col min="13" max="15" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>3</v>
@@ -1699,40 +1718,37 @@
         <v>5</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>34</v>
+        <v>70</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>35</v>
+        <v>6</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>6</v>
+        <v>46</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>50</v>
+        <v>14</v>
       </c>
       <c r="J1" s="7" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="K1" s="7" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="L1" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="M1" s="7" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="N1" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="O1" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>29</v>
       </c>
@@ -1743,35 +1759,36 @@
         <v>12</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="1"/>
+        <v>57</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="H2" s="1" t="s">
-        <v>31</v>
+        <v>71</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>41</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="K2" s="1"/>
       <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
+      <c r="M2" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="N2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="O2" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>30</v>
       </c>
@@ -1782,31 +1799,32 @@
         <v>13</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
+        <v>57</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="H3" s="1" t="s">
-        <v>31</v>
+        <v>72</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>42</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="K3" s="1"/>
       <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
+      <c r="M3" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="N3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="O3" s="1" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1820,8 +1838,206 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD8FB4E8-B9B5-D24A-91D9-6FACBB875664}">
+  <dimension ref="A1:L7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="17.83203125" customWidth="1"/>
+    <col min="8" max="8" width="22" customWidth="1"/>
+    <col min="9" max="9" width="15.83203125" customWidth="1"/>
+    <col min="10" max="10" width="22.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="K1" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1">
+        <v>100</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1">
+        <v>100</v>
+      </c>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1">
+        <v>100</v>
+      </c>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1">
+        <v>100</v>
+      </c>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FCD209A-28DD-7845-952F-4118CB029C17}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1842,21 +2058,21 @@
         <v>4</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>29</v>
@@ -1873,7 +2089,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>29</v>
@@ -1882,151 +2098,46 @@
         <v>27</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E5" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD8FB4E8-B9B5-D24A-91D9-6FACBB875664}">
-  <dimension ref="A1:J4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="15.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="8" max="8" width="22" customWidth="1"/>
-    <col min="9" max="9" width="15.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="G1" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="I1" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="J1" s="11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1">
-        <v>100</v>
-      </c>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1">
-        <v>100</v>
-      </c>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E6" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2053,10 +2164,10 @@
         <v>4</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
updated mac version to 0.0.0.0.19
</commit_message>
<xml_diff>
--- a/examples/vpc.xlsx
+++ b/examples/vpc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jww/Developer/python/terraformer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{850EC2E4-B4DE-A84D-9A26-3CE3946DA39C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0806254C-5D2E-4C48-A97A-B6855BFEB9DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="480" windowWidth="25600" windowHeight="14700" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="vpcheaders" sheetId="6" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="77">
   <si>
     <t>public_gateway</t>
   </si>
@@ -253,13 +253,22 @@
     <t>boot_volume</t>
   </si>
   <si>
-    <t>vsi1primarynic</t>
-  </si>
-  <si>
-    <t>vsi2primarynic</t>
-  </si>
-  <si>
     <t>general-purpose</t>
+  </si>
+  <si>
+    <t>*interface_type</t>
+  </si>
+  <si>
+    <t>primary</t>
+  </si>
+  <si>
+    <t>secondary</t>
+  </si>
+  <si>
+    <t>vsi1nic0</t>
+  </si>
+  <si>
+    <t>vsi2nic0</t>
   </si>
 </sst>
 </file>
@@ -415,7 +424,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="74">
+  <dxfs count="75">
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -435,6 +444,9 @@
           <bgColor theme="4"/>
         </patternFill>
       </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1004,13 +1016,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{7215B7F5-B70C-6B42-84D7-6729B99B446D}" name="Table8" displayName="Table8" ref="A1:F3" totalsRowShown="0" headerRowDxfId="73" dataDxfId="72" tableBorderDxfId="71">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{7215B7F5-B70C-6B42-84D7-6729B99B446D}" name="Table8" displayName="Table8" ref="A1:F3" totalsRowShown="0" headerRowDxfId="74" dataDxfId="73" tableBorderDxfId="72">
   <autoFilter ref="A1:F3" xr:uid="{529F7172-ECCA-724F-9B2D-5A6C4B69CB3C}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{887BA8C8-9946-8A42-98DF-3633CAED0C28}" name="*name" dataDxfId="70"/>
-    <tableColumn id="5" xr3:uid="{5CEDAE6E-6D63-FE4C-B1E4-8EBD674619A5}" name="default_network_acl" dataDxfId="69"/>
+    <tableColumn id="1" xr3:uid="{887BA8C8-9946-8A42-98DF-3633CAED0C28}" name="*name" dataDxfId="71"/>
+    <tableColumn id="5" xr3:uid="{5CEDAE6E-6D63-FE4C-B1E4-8EBD674619A5}" name="default_network_acl" dataDxfId="70"/>
     <tableColumn id="3" xr3:uid="{D2048242-D53A-2A48-924A-8019052FD266}" name="address_prefix_management"/>
-    <tableColumn id="2" xr3:uid="{A41B6291-1C2E-AB41-A22B-93622DC498B2}" name="classic_access" dataDxfId="68"/>
+    <tableColumn id="2" xr3:uid="{A41B6291-1C2E-AB41-A22B-93622DC498B2}" name="classic_access" dataDxfId="69"/>
     <tableColumn id="4" xr3:uid="{9675255E-64F1-104E-BCF2-8AF88D430E4B}" name="resource_group"/>
     <tableColumn id="7" xr3:uid="{DF1FC027-D537-CB40-BAA8-AEAEE8D9E2C7}" name="tags"/>
   </tableColumns>
@@ -1019,102 +1031,103 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{80420FF8-12AA-D148-A5E9-F305380E9AC4}" name="Table82" displayName="Table82" ref="A1:D3" totalsRowShown="0" headerRowDxfId="67" dataDxfId="66" tableBorderDxfId="65">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{80420FF8-12AA-D148-A5E9-F305380E9AC4}" name="Table82" displayName="Table82" ref="A1:D3" totalsRowShown="0" headerRowDxfId="68" dataDxfId="67" tableBorderDxfId="66">
   <autoFilter ref="A1:D3" xr:uid="{9C9BAFE8-9631-CE45-93B1-83DB9C4014D5}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{C6C9ADE6-AC77-4944-9C6C-9D136392888D}" name="*name" dataDxfId="64"/>
-    <tableColumn id="5" xr3:uid="{0731D78F-C6D2-8948-BD0A-FB61D3B47F6C}" name="*vpc" dataDxfId="63"/>
+    <tableColumn id="1" xr3:uid="{C6C9ADE6-AC77-4944-9C6C-9D136392888D}" name="*name" dataDxfId="65"/>
+    <tableColumn id="5" xr3:uid="{0731D78F-C6D2-8948-BD0A-FB61D3B47F6C}" name="*vpc" dataDxfId="64"/>
     <tableColumn id="3" xr3:uid="{A408C4C2-23CE-B443-BA1D-7440072D5651}" name="*zone"/>
-    <tableColumn id="2" xr3:uid="{F0825E63-100E-584C-B142-E4481E9F997C}" name="*cidr" dataDxfId="62"/>
+    <tableColumn id="2" xr3:uid="{F0825E63-100E-584C-B142-E4481E9F997C}" name="*cidr" dataDxfId="63"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{E7E4E482-6BB9-E248-AF8D-C5304BC1A44F}" name="Table3236" displayName="Table3236" ref="A1:E3" totalsRowShown="0" headerRowDxfId="61" dataDxfId="60">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{E7E4E482-6BB9-E248-AF8D-C5304BC1A44F}" name="Table3236" displayName="Table3236" ref="A1:E3" totalsRowShown="0" headerRowDxfId="62" dataDxfId="61">
   <autoFilter ref="A1:E3" xr:uid="{DC08D300-10E5-4A45-A724-480E99186CDC}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{60C065E1-55B2-104C-9BD3-648FFAC30A51}" name="*name" dataDxfId="59"/>
-    <tableColumn id="3" xr3:uid="{8BD05EA0-AFD7-AF41-B934-9ECEE2438312}" name="*vpc" dataDxfId="58"/>
-    <tableColumn id="2" xr3:uid="{92355D65-8FB2-FA47-80DC-D34EF9FEADBD}" name="*zone" dataDxfId="57"/>
-    <tableColumn id="4" xr3:uid="{EF21D846-0B2C-9441-B0FD-2EA28736C729}" name="*destination" dataDxfId="56"/>
-    <tableColumn id="5" xr3:uid="{7D2B7989-C527-9D46-A034-89A1FB4BA0D5}" name="*next_hop" dataDxfId="55"/>
+    <tableColumn id="1" xr3:uid="{60C065E1-55B2-104C-9BD3-648FFAC30A51}" name="*name" dataDxfId="60"/>
+    <tableColumn id="3" xr3:uid="{8BD05EA0-AFD7-AF41-B934-9ECEE2438312}" name="*vpc" dataDxfId="59"/>
+    <tableColumn id="2" xr3:uid="{92355D65-8FB2-FA47-80DC-D34EF9FEADBD}" name="*zone" dataDxfId="58"/>
+    <tableColumn id="4" xr3:uid="{EF21D846-0B2C-9441-B0FD-2EA28736C729}" name="*destination" dataDxfId="57"/>
+    <tableColumn id="5" xr3:uid="{7D2B7989-C527-9D46-A034-89A1FB4BA0D5}" name="*next_hop" dataDxfId="56"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{76790F31-1453-B641-9754-80A9D247EA0F}" name="Table6" displayName="Table6" ref="A1:K3" totalsRowShown="0" headerRowDxfId="54" dataDxfId="53">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{76790F31-1453-B641-9754-80A9D247EA0F}" name="Table6" displayName="Table6" ref="A1:K3" totalsRowShown="0" headerRowDxfId="55" dataDxfId="54">
   <autoFilter ref="A1:K3" xr:uid="{9725F296-5A96-A949-A782-B4A2B65596C4}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{1E9E58AF-C46F-2140-86A4-81396AD00F15}" name="*name" dataDxfId="52"/>
-    <tableColumn id="11" xr3:uid="{9C2673D8-AB9A-9645-A3ED-D9B779022434}" name="*vpc" dataDxfId="51"/>
-    <tableColumn id="2" xr3:uid="{D989FA97-121E-ED4E-9CA5-25D303F38C24}" name="*zone" dataDxfId="50"/>
-    <tableColumn id="3" xr3:uid="{9DE77DE5-F660-7D4C-BC60-2B014D5E01EB}" name="ipv4_cidr_block" dataDxfId="49"/>
-    <tableColumn id="4" xr3:uid="{42D706D7-A721-6D49-8189-9A181B88E99F}" name="total_ipv4_address_count" dataDxfId="48"/>
-    <tableColumn id="5" xr3:uid="{215941D8-E315-5044-8E51-E2FEE9B95908}" name="ip_version" dataDxfId="47"/>
-    <tableColumn id="6" xr3:uid="{7CE7912A-5366-5A4D-9CAD-006BE9E02B39}" name="network_acl" dataDxfId="46"/>
-    <tableColumn id="7" xr3:uid="{87A1EA58-5C4B-0443-A650-07ABED9C6F31}" name="public_gateway" dataDxfId="45"/>
-    <tableColumn id="8" xr3:uid="{718DFD83-0842-7749-8498-7034DCF9F245}" name="create_timeout" dataDxfId="44"/>
-    <tableColumn id="9" xr3:uid="{6E310B89-982B-B743-8106-2EEBD001DB52}" name="update_timeout" dataDxfId="43"/>
-    <tableColumn id="10" xr3:uid="{16A0C085-1B24-8740-BCEF-FC5FBADEF6C0}" name="delete_timeout" dataDxfId="42"/>
+    <tableColumn id="1" xr3:uid="{1E9E58AF-C46F-2140-86A4-81396AD00F15}" name="*name" dataDxfId="53"/>
+    <tableColumn id="11" xr3:uid="{9C2673D8-AB9A-9645-A3ED-D9B779022434}" name="*vpc" dataDxfId="52"/>
+    <tableColumn id="2" xr3:uid="{D989FA97-121E-ED4E-9CA5-25D303F38C24}" name="*zone" dataDxfId="51"/>
+    <tableColumn id="3" xr3:uid="{9DE77DE5-F660-7D4C-BC60-2B014D5E01EB}" name="ipv4_cidr_block" dataDxfId="50"/>
+    <tableColumn id="4" xr3:uid="{42D706D7-A721-6D49-8189-9A181B88E99F}" name="total_ipv4_address_count" dataDxfId="49"/>
+    <tableColumn id="5" xr3:uid="{215941D8-E315-5044-8E51-E2FEE9B95908}" name="ip_version" dataDxfId="48"/>
+    <tableColumn id="6" xr3:uid="{7CE7912A-5366-5A4D-9CAD-006BE9E02B39}" name="network_acl" dataDxfId="47"/>
+    <tableColumn id="7" xr3:uid="{87A1EA58-5C4B-0443-A650-07ABED9C6F31}" name="public_gateway" dataDxfId="46"/>
+    <tableColumn id="8" xr3:uid="{718DFD83-0842-7749-8498-7034DCF9F245}" name="create_timeout" dataDxfId="45"/>
+    <tableColumn id="9" xr3:uid="{6E310B89-982B-B743-8106-2EEBD001DB52}" name="update_timeout" dataDxfId="44"/>
+    <tableColumn id="10" xr3:uid="{16A0C085-1B24-8740-BCEF-FC5FBADEF6C0}" name="delete_timeout" dataDxfId="43"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{3F1E4605-7351-6A4A-9807-A10DCEAD79B7}" name="Table7" displayName="Table7" ref="A1:N3" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{3F1E4605-7351-6A4A-9807-A10DCEAD79B7}" name="Table7" displayName="Table7" ref="A1:N3" totalsRowShown="0" headerRowDxfId="42" dataDxfId="41">
   <autoFilter ref="A1:N3" xr:uid="{4F0FA061-E3B2-AB4E-A276-92C803DED60C}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{B447E9AB-445F-0242-8396-EEAA92074797}" name="*name" dataDxfId="39"/>
-    <tableColumn id="7" xr3:uid="{AECA3B2B-972B-2947-B76F-3FE48277F64A}" name="*vpc" dataDxfId="38"/>
-    <tableColumn id="2" xr3:uid="{E6843232-FC96-094F-809F-D9A2D9A3F5CB}" name="*zone" dataDxfId="37"/>
-    <tableColumn id="3" xr3:uid="{E7DB5053-DB66-CF46-AB33-5A411FF07264}" name="*profile" dataDxfId="36"/>
-    <tableColumn id="4" xr3:uid="{F65626CD-0D0E-D748-9934-00DB105BEEAC}" name="*image" dataDxfId="35"/>
-    <tableColumn id="14" xr3:uid="{1A5FD37C-8F61-7B49-9DE5-C024F0CC91E5}" name="boot_volume" dataDxfId="34"/>
-    <tableColumn id="6" xr3:uid="{FFE24952-72F9-9D47-8A4B-2813BCCB260E}" name="*keys" dataDxfId="33"/>
-    <tableColumn id="9" xr3:uid="{A03604D8-6E33-4249-A9DE-BF8870E3D90B}" name="*primary_network_interface" dataDxfId="32"/>
-    <tableColumn id="10" xr3:uid="{438F95E2-E2D5-1E49-9852-4B915078693E}" name="network_interfaces" dataDxfId="31"/>
-    <tableColumn id="19" xr3:uid="{6293540A-4A05-0E4A-99ED-C75D3F46ECCF}" name="volumes" dataDxfId="30"/>
-    <tableColumn id="18" xr3:uid="{8C2D6431-BD15-6849-BBE1-C0EF1B26E51A}" name="user_data" dataDxfId="29"/>
-    <tableColumn id="17" xr3:uid="{8C7E9F80-830B-174D-9411-54916978023E}" name="resource_group" dataDxfId="28"/>
-    <tableColumn id="12" xr3:uid="{E2511928-0801-3546-B6BA-F9C8EF98BBC6}" name="create_timeout" dataDxfId="27"/>
-    <tableColumn id="13" xr3:uid="{F33A3F16-B62A-EC4B-BC5D-BAA56655B743}" name="delete_timeout" dataDxfId="26"/>
+    <tableColumn id="1" xr3:uid="{B447E9AB-445F-0242-8396-EEAA92074797}" name="*name" dataDxfId="40"/>
+    <tableColumn id="7" xr3:uid="{AECA3B2B-972B-2947-B76F-3FE48277F64A}" name="*vpc" dataDxfId="39"/>
+    <tableColumn id="2" xr3:uid="{E6843232-FC96-094F-809F-D9A2D9A3F5CB}" name="*zone" dataDxfId="38"/>
+    <tableColumn id="3" xr3:uid="{E7DB5053-DB66-CF46-AB33-5A411FF07264}" name="*profile" dataDxfId="37"/>
+    <tableColumn id="4" xr3:uid="{F65626CD-0D0E-D748-9934-00DB105BEEAC}" name="*image" dataDxfId="36"/>
+    <tableColumn id="14" xr3:uid="{1A5FD37C-8F61-7B49-9DE5-C024F0CC91E5}" name="boot_volume" dataDxfId="35"/>
+    <tableColumn id="6" xr3:uid="{FFE24952-72F9-9D47-8A4B-2813BCCB260E}" name="*keys" dataDxfId="34"/>
+    <tableColumn id="9" xr3:uid="{A03604D8-6E33-4249-A9DE-BF8870E3D90B}" name="*primary_network_interface" dataDxfId="33"/>
+    <tableColumn id="10" xr3:uid="{438F95E2-E2D5-1E49-9852-4B915078693E}" name="network_interfaces" dataDxfId="32"/>
+    <tableColumn id="19" xr3:uid="{6293540A-4A05-0E4A-99ED-C75D3F46ECCF}" name="volumes" dataDxfId="31"/>
+    <tableColumn id="18" xr3:uid="{8C2D6431-BD15-6849-BBE1-C0EF1B26E51A}" name="user_data" dataDxfId="30"/>
+    <tableColumn id="17" xr3:uid="{8C7E9F80-830B-174D-9411-54916978023E}" name="resource_group" dataDxfId="29"/>
+    <tableColumn id="12" xr3:uid="{E2511928-0801-3546-B6BA-F9C8EF98BBC6}" name="create_timeout" dataDxfId="28"/>
+    <tableColumn id="13" xr3:uid="{F33A3F16-B62A-EC4B-BC5D-BAA56655B743}" name="delete_timeout" dataDxfId="27"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C451A855-5250-674B-8039-E23EC3348E96}" name="Table11" displayName="Table11" ref="A1:L6" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C451A855-5250-674B-8039-E23EC3348E96}" name="Table11" displayName="Table11" ref="A1:L6" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
   <autoFilter ref="A1:L6" xr:uid="{8CD156A6-A66F-1245-BCD2-9FAE26A0A77C}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{CDC18A34-D228-8E41-90CD-62AD9ACAF229}" name="*name" dataDxfId="23"/>
-    <tableColumn id="11" xr3:uid="{314C1371-3329-EA42-AB4C-3D8F83971269}" name="*instance" dataDxfId="22"/>
-    <tableColumn id="12" xr3:uid="{1BF2A89E-63CD-FA4D-B1ED-9A3CD987DFF3}" name="*attachment_type" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{480E110A-7DA0-1A46-B19A-DAB8291BA972}" name="*zone" dataDxfId="20"/>
-    <tableColumn id="3" xr3:uid="{1B453B9B-A3A5-5948-96F3-62C87F788C3A}" name="*profile" dataDxfId="19"/>
-    <tableColumn id="4" xr3:uid="{6CC60290-7B72-D343-A43F-F0F762500CF4}" name="iops" dataDxfId="18"/>
-    <tableColumn id="5" xr3:uid="{45C880C0-FF4F-2F4A-919A-124DB93E5010}" name="capacity" dataDxfId="17"/>
-    <tableColumn id="6" xr3:uid="{787D8375-0B24-5F42-A273-3093BD8B60EC}" name="encryption_key" dataDxfId="16"/>
-    <tableColumn id="7" xr3:uid="{392944E6-6831-6F41-86DE-438B3577B0C6}" name="resource_group" dataDxfId="15"/>
-    <tableColumn id="8" xr3:uid="{2D73C361-1CE6-FF4D-BC45-651F77AC5BE1}" name="resource_controller_url" dataDxfId="14"/>
-    <tableColumn id="9" xr3:uid="{DC38DEC2-7381-DD45-A09D-F3050D08CA1E}" name="create_timeout" dataDxfId="13"/>
-    <tableColumn id="10" xr3:uid="{63225B45-4949-7A45-9F18-531EB8888D63}" name="delete_timeout" dataDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{CDC18A34-D228-8E41-90CD-62AD9ACAF229}" name="*name" dataDxfId="24"/>
+    <tableColumn id="11" xr3:uid="{314C1371-3329-EA42-AB4C-3D8F83971269}" name="*instance" dataDxfId="23"/>
+    <tableColumn id="12" xr3:uid="{1BF2A89E-63CD-FA4D-B1ED-9A3CD987DFF3}" name="*attachment_type" dataDxfId="22"/>
+    <tableColumn id="2" xr3:uid="{480E110A-7DA0-1A46-B19A-DAB8291BA972}" name="*zone" dataDxfId="21"/>
+    <tableColumn id="3" xr3:uid="{1B453B9B-A3A5-5948-96F3-62C87F788C3A}" name="*profile" dataDxfId="20"/>
+    <tableColumn id="4" xr3:uid="{6CC60290-7B72-D343-A43F-F0F762500CF4}" name="iops" dataDxfId="19"/>
+    <tableColumn id="5" xr3:uid="{45C880C0-FF4F-2F4A-919A-124DB93E5010}" name="capacity" dataDxfId="18"/>
+    <tableColumn id="6" xr3:uid="{787D8375-0B24-5F42-A273-3093BD8B60EC}" name="encryption_key" dataDxfId="17"/>
+    <tableColumn id="7" xr3:uid="{392944E6-6831-6F41-86DE-438B3577B0C6}" name="resource_group" dataDxfId="16"/>
+    <tableColumn id="8" xr3:uid="{2D73C361-1CE6-FF4D-BC45-651F77AC5BE1}" name="resource_controller_url" dataDxfId="15"/>
+    <tableColumn id="9" xr3:uid="{DC38DEC2-7381-DD45-A09D-F3050D08CA1E}" name="create_timeout" dataDxfId="14"/>
+    <tableColumn id="10" xr3:uid="{63225B45-4949-7A45-9F18-531EB8888D63}" name="delete_timeout" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{81661C9C-F36C-2E41-BF2C-12573A860276}" name="Table75" displayName="Table75" ref="A1:E6" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:E6" xr:uid="{4F0FA061-E3B2-AB4E-A276-92C803DED60C}"/>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{95E267F3-7620-8C4D-AFC7-4EB9DFAE946B}" name="*name" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{C13CAAAB-1F09-F442-B06D-36989DBA835A}" name="*instance" dataDxfId="8"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{81661C9C-F36C-2E41-BF2C-12573A860276}" name="Table75" displayName="Table75" ref="A1:F6" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+  <autoFilter ref="A1:F6" xr:uid="{4F0FA061-E3B2-AB4E-A276-92C803DED60C}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{95E267F3-7620-8C4D-AFC7-4EB9DFAE946B}" name="*name" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{C13CAAAB-1F09-F442-B06D-36989DBA835A}" name="*instance" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{3B52CA6E-776E-904A-AD7B-C6EF3697A5C1}" name="*interface_type" dataDxfId="8"/>
     <tableColumn id="8" xr3:uid="{B55BB537-FA6A-D04D-99CC-63555EFADEB6}" name="*subnet" dataDxfId="7"/>
     <tableColumn id="11" xr3:uid="{346BFF31-BC5B-C647-89BB-72AE7861274F}" name="security_groups" dataDxfId="6"/>
     <tableColumn id="7" xr3:uid="{80D936B9-9EFA-6C4B-BF5E-9435B5B9B191}" name="floating_ip" dataDxfId="5"/>
@@ -1400,7 +1413,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D5606E7-1677-4EE2-808E-F237A1A9F8B6}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1689,7 +1702,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69A31708-3A2C-4ADA-B3E5-8A1B18923F2A}">
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1771,7 +1784,7 @@
         <v>31</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>39</v>
@@ -1811,7 +1824,7 @@
         <v>31</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>40</v>
@@ -1903,7 +1916,7 @@
         <v>12</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1">
@@ -1973,7 +1986,7 @@
         <v>13</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1">
@@ -2037,9 +2050,11 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FCD209A-28DD-7845-952F-4118CB029C17}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2053,41 +2068,47 @@
     <col min="13" max="15" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="F1" s="7" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>29</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>39</v>
       </c>
@@ -2095,36 +2116,43 @@
         <v>29</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="1"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>40</v>
       </c>
@@ -2132,12 +2160,15 @@
         <v>30</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>